<commit_message>
docs: update revenue, additional refund $174 from china mobile.
</commit_message>
<xml_diff>
--- a/Alan Tang_s Income Expense Future.xlsx
+++ b/Alan Tang_s Income Expense Future.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Income-Expenditure-Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111186A2-68E3-4ADE-9CC4-494BD5DC3C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF23421-B929-41DD-BC5B-19C87D4A80B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="April 2024 - June 2024" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="375">
   <si>
     <t>Assets</t>
   </si>
@@ -1293,6 +1293,12 @@
   </si>
   <si>
     <t>Receive $100 HKD from Lawrence, no need to return back</t>
+  </si>
+  <si>
+    <t>China Mobile Refund</t>
+  </si>
+  <si>
+    <t>Refund the excess Fees For Joox</t>
   </si>
 </sst>
 </file>
@@ -4144,8 +4150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1053"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4244,14 +4250,14 @@
         <v>76</v>
       </c>
       <c r="C4" s="4">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
         <v>76</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="94" t="s">
@@ -4284,7 +4290,7 @@
         <v>77</v>
       </c>
       <c r="C5" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
@@ -4458,8 +4464,8 @@
         <v>337</v>
       </c>
       <c r="I9" s="95">
-        <f>'October 2024 - December 2024'!E92</f>
-        <v>747.01000000000022</v>
+        <f>'October 2024 - December 2024'!E93</f>
+        <v>921.01000000000022</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -4498,8 +4504,8 @@
         <v>173</v>
       </c>
       <c r="I10" s="95">
-        <f>'October 2024 - December 2024'!E101</f>
-        <v>875.01000000000022</v>
+        <f>'October 2024 - December 2024'!E102</f>
+        <v>1049.0100000000002</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -4525,7 +4531,7 @@
       </c>
       <c r="C11" s="4">
         <f>SUM(C3:C10)</f>
-        <v>518.01</v>
+        <v>499.01</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="62" t="s">
@@ -4533,15 +4539,15 @@
       </c>
       <c r="F11" s="55">
         <f>SUM(F3:F10)</f>
-        <v>418.01</v>
+        <v>518.01</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="94" t="s">
         <v>174</v>
       </c>
       <c r="I11" s="95">
-        <f>'October 2024 - December 2024'!E110</f>
-        <v>903.01000000000022</v>
+        <f>'October 2024 - December 2024'!E111</f>
+        <v>1077.0100000000002</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -4578,7 +4584,7 @@
       </c>
       <c r="I12" s="95">
         <f>'January 2025 - March 2025'!E89</f>
-        <v>931.01000000000022</v>
+        <v>1105.0100000000002</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -4610,7 +4616,7 @@
       </c>
       <c r="I13" s="95">
         <f>'January 2025 - March 2025'!E97</f>
-        <v>959.01000000000022</v>
+        <v>1133.0100000000002</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -4635,7 +4641,7 @@
       </c>
       <c r="I14" s="95">
         <f>'January 2025 - March 2025'!E106</f>
-        <v>987.01000000000022</v>
+        <v>1161.0100000000002</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="30" customHeight="1">
@@ -4652,7 +4658,7 @@
       </c>
       <c r="I15" s="95">
         <f>'April 2025 - June 2025'!E89</f>
-        <v>815.01000000000022</v>
+        <v>989.01000000000022</v>
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
@@ -4690,7 +4696,7 @@
       </c>
       <c r="I16" s="95">
         <f>'April 2025 - June 2025'!E97</f>
-        <v>643.01000000000022</v>
+        <v>817.01000000000022</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="30" customHeight="1">
@@ -4712,7 +4718,7 @@
       </c>
       <c r="I17" s="95">
         <f>'April 2025 - June 2025'!E106</f>
-        <v>471.01000000000022</v>
+        <v>645.01000000000022</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="30" customHeight="1">
@@ -4731,7 +4737,7 @@
       </c>
       <c r="I18" s="95">
         <f>'July 2025 - September 2025'!E89</f>
-        <v>1299.0100000000002</v>
+        <v>1473.0100000000002</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="30" customHeight="1">
@@ -4742,7 +4748,7 @@
       </c>
       <c r="I19" s="95">
         <f>'July 2025 - September 2025'!E97</f>
-        <v>2127.0100000000002</v>
+        <v>2301.0100000000002</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="30" customHeight="1">
@@ -4759,7 +4765,7 @@
       </c>
       <c r="I20" s="95">
         <f>'July 2025 - September 2025'!E106</f>
-        <v>2955.01</v>
+        <v>3129.01</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
@@ -4798,7 +4804,7 @@
       </c>
       <c r="I21" s="95">
         <f>'October 2025 - December 2025'!E89</f>
-        <v>3783.01</v>
+        <v>3957.01</v>
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
@@ -4837,7 +4843,7 @@
       </c>
       <c r="I22" s="95">
         <f>'October 2025 - December 2025'!E97</f>
-        <v>4611.01</v>
+        <v>4785.01</v>
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
@@ -4876,7 +4882,7 @@
       </c>
       <c r="I23" s="125">
         <f>'October 2025 - December 2025'!E106</f>
-        <v>5439.01</v>
+        <v>5613.01</v>
       </c>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
@@ -4929,7 +4935,7 @@
       </c>
       <c r="I25" s="95">
         <f>'January 2026 - March 2026'!E89</f>
-        <v>6267.01</v>
+        <v>6441.01</v>
       </c>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
@@ -4960,7 +4966,7 @@
       </c>
       <c r="I26" s="95">
         <f>'January 2026 - March 2026'!E97</f>
-        <v>7095.01</v>
+        <v>7269.01</v>
       </c>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
@@ -4991,7 +4997,7 @@
       </c>
       <c r="I27" s="95">
         <f>'January 2026 - March 2026'!E106</f>
-        <v>7923.01</v>
+        <v>8097.01</v>
       </c>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
@@ -5024,7 +5030,7 @@
       </c>
       <c r="I28" s="95">
         <f>'April 2026 - June 2026'!E89</f>
-        <v>8751.01</v>
+        <v>8925.01</v>
       </c>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
@@ -5063,7 +5069,7 @@
       </c>
       <c r="I29" s="147">
         <f>'April 2026 - June 2026'!E97</f>
-        <v>9579.01</v>
+        <v>9753.01</v>
       </c>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
@@ -5128,7 +5134,7 @@
       </c>
       <c r="I32" s="95">
         <f>'April 2026 - June 2026'!E106</f>
-        <v>10407.01</v>
+        <v>10581.01</v>
       </c>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
@@ -10092,8 +10098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5F3FA5-5013-4B35-A74B-6269617B858B}">
   <dimension ref="A1:Y1051"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -11562,7 +11568,7 @@
         <v>355</v>
       </c>
       <c r="H128" s="118">
-        <v>144.5</v>
+        <v>163.5</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="60">
@@ -11582,7 +11588,7 @@
       </c>
       <c r="H129" s="117">
         <f>330-H128</f>
-        <v>185.5</v>
+        <v>166.5</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="13.5" customHeight="1">
@@ -15496,10 +15502,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1EAFDB-34A9-4E8B-8792-A6B6BA3CC3A2}">
-  <dimension ref="A1:Y1023"/>
+  <dimension ref="A1:Y1024"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -15544,8 +15550,8 @@
         <v>138</v>
       </c>
       <c r="C3" s="4">
-        <f>E110</f>
-        <v>903.01000000000022</v>
+        <f>E111</f>
+        <v>1077.0100000000002</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -15577,7 +15583,7 @@
       </c>
       <c r="C4" s="55">
         <f>SUM(C3:C3)</f>
-        <v>903.01000000000022</v>
+        <v>1077.0100000000002</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -15608,7 +15614,7 @@
         <v>110</v>
       </c>
       <c r="C5" s="55">
-        <f>C81</f>
+        <f>C82</f>
         <v>-5400</v>
       </c>
       <c r="D5" s="5"/>
@@ -15735,229 +15741,235 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:25" ht="17.25" customHeight="1">
+      <c r="A12" s="32"/>
+      <c r="B12" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="C12" s="246" t="s">
+        <v>374</v>
+      </c>
+      <c r="D12" s="260"/>
+      <c r="E12" s="65">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A13" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B13" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="221" t="s">
+      <c r="C13" s="221" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="222"/>
-      <c r="E12" s="65">
+      <c r="D13" s="222"/>
+      <c r="E13" s="65">
         <v>2405</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="47">
-        <f>SUM(E10:E12)</f>
-        <v>2483</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="13.5" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="47">
+        <f>SUM(E10:E13)</f>
+        <v>2657</v>
+      </c>
     </row>
     <row r="15" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A15" s="226" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:25" ht="13.5" customHeight="1">
+      <c r="A16" s="226" t="s">
         <v>288</v>
       </c>
-      <c r="B15" s="192"/>
-      <c r="C15" s="192"/>
-      <c r="D15" s="192"/>
-      <c r="E15" s="193"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
-      <c r="Y15" s="13"/>
-    </row>
-    <row r="16" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A16" s="14" t="s">
+      <c r="B16" s="192"/>
+      <c r="C16" s="192"/>
+      <c r="D16" s="192"/>
+      <c r="E16" s="193"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+    </row>
+    <row r="17" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A17" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B17" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="227" t="s">
+      <c r="C17" s="227" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="162"/>
-      <c r="E16" s="16" t="s">
+      <c r="D17" s="162"/>
+      <c r="E17" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A17" s="24" t="s">
+    <row r="18" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A18" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="224" t="s">
+      <c r="C18" s="224" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="162"/>
-      <c r="E17" s="18">
+      <c r="D18" s="162"/>
+      <c r="E18" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A18" s="32" t="s">
+    <row r="19" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A19" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B19" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="221" t="s">
+      <c r="C19" s="221" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="222"/>
-      <c r="E18" s="65">
+      <c r="D19" s="222"/>
+      <c r="E19" s="65">
         <v>2405</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="12">
-        <f>SUM(E17,E18)</f>
-        <v>2405</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" ht="13.5" customHeight="1">
+    <row r="20" spans="1:25" ht="13.15" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="50"/>
+      <c r="D20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="12">
+        <f>SUM(E18,E19)</f>
+        <v>2405</v>
+      </c>
     </row>
     <row r="21" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A21" s="226" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="50"/>
+    </row>
+    <row r="22" spans="1:25" ht="13.5" customHeight="1">
+      <c r="A22" s="226" t="s">
         <v>295</v>
       </c>
-      <c r="B21" s="192"/>
-      <c r="C21" s="192"/>
-      <c r="D21" s="192"/>
-      <c r="E21" s="193"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
-      <c r="Y21" s="13"/>
-    </row>
-    <row r="22" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A22" s="68" t="s">
+      <c r="B22" s="192"/>
+      <c r="C22" s="192"/>
+      <c r="D22" s="192"/>
+      <c r="E22" s="193"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+    </row>
+    <row r="23" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A23" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="69" t="s">
+      <c r="B23" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="244" t="s">
+      <c r="C23" s="244" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="215"/>
-      <c r="E22" s="70" t="s">
+      <c r="D23" s="215"/>
+      <c r="E23" s="70" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A23" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="150" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="245"/>
-      <c r="E23" s="65">
-        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="13.15" customHeight="1">
       <c r="A24" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="150" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="245"/>
+      <c r="E24" s="65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A25" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B25" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="221" t="s">
+      <c r="C25" s="221" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="222"/>
-      <c r="E24" s="65">
+      <c r="D25" s="222"/>
+      <c r="E25" s="65">
         <v>2405</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A25" s="44"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="46" t="s">
+    <row r="26" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="47">
-        <f>SUM(E23:E24)</f>
+      <c r="E26" s="47">
+        <f>SUM(E24:E25)</f>
         <v>2405</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="50"/>
-    </row>
-    <row r="27" spans="1:25" ht="13.15" customHeight="1">
+    <row r="27" spans="1:25" ht="13.5" customHeight="1">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="1"/>
       <c r="D27" s="49"/>
       <c r="E27" s="50"/>
     </row>
-    <row r="28" spans="1:25" ht="13.5" customHeight="1">
+    <row r="28" spans="1:25" ht="13.15" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="1"/>
@@ -15967,105 +15979,103 @@
     <row r="29" spans="1:25" ht="13.5" customHeight="1">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="50"/>
     </row>
     <row r="30" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A30" s="243" t="s">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:25" ht="13.5" customHeight="1">
+      <c r="A31" s="243" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="161"/>
-      <c r="C30" s="162"/>
-    </row>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A31" s="19" t="s">
+      <c r="B31" s="161"/>
+      <c r="C31" s="162"/>
+    </row>
+    <row r="32" spans="1:25" ht="13.5" customHeight="1">
+      <c r="A32" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B32" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C32" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="21"/>
-    </row>
-    <row r="32" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A32" s="163" t="s">
+      <c r="D32" s="21"/>
+    </row>
+    <row r="33" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A33" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="161"/>
-      <c r="C32" s="162"/>
-    </row>
-    <row r="33" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A33" s="24" t="s">
+      <c r="B33" s="161"/>
+      <c r="C33" s="162"/>
+    </row>
+    <row r="34" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A34" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="18">
+      <c r="B34" s="2"/>
+      <c r="C34" s="18">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A34" s="29" t="s">
+    <row r="35" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A35" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="26">
+      <c r="B35" s="25"/>
+      <c r="C35" s="26">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A35" s="25" t="s">
+    <row r="36" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A36" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B36" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C36" s="26">
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A36" s="27"/>
-      <c r="B36" s="24" t="s">
+    <row r="37" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A37" s="27"/>
+      <c r="B37" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="28">
-        <f>SUM(C33:C35)</f>
+      <c r="C37" s="28">
+        <f>SUM(C34:C36)</f>
         <v>227</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A37" s="207" t="s">
+    <row r="38" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A38" s="207" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="208"/>
-      <c r="C37" s="209"/>
-    </row>
-    <row r="38" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A38" s="210"/>
-      <c r="B38" s="211"/>
-      <c r="C38" s="212"/>
+      <c r="B38" s="208"/>
+      <c r="C38" s="209"/>
     </row>
     <row r="39" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="17">
-        <v>0</v>
-      </c>
+      <c r="A39" s="210"/>
+      <c r="B39" s="211"/>
+      <c r="C39" s="212"/>
     </row>
     <row r="40" spans="1:3" ht="13.5" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="C40" s="9">
+      <c r="C40" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="13.5" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="9">
@@ -16074,7 +16084,7 @@
     </row>
     <row r="42" spans="1:3" ht="13.5" customHeight="1">
       <c r="A42" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="9">
@@ -16083,7 +16093,7 @@
     </row>
     <row r="43" spans="1:3" ht="13.5" customHeight="1">
       <c r="A43" s="2" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="9">
@@ -16091,85 +16101,85 @@
       </c>
     </row>
     <row r="44" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2" t="s">
+      <c r="A44" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C44" s="9">
-        <f>SUM(C39:C43)</f>
+      <c r="C45" s="9">
+        <f>SUM(C40:C44)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A45" s="163" t="s">
+    <row r="46" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A46" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="161"/>
-      <c r="C45" s="162"/>
-    </row>
-    <row r="46" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A46" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" s="18">
-        <v>0</v>
-      </c>
+      <c r="B46" s="161"/>
+      <c r="C46" s="162"/>
     </row>
     <row r="47" spans="1:3" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C47" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A48" s="2"/>
-      <c r="B48" s="24" t="s">
+      <c r="A48" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C48" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A49" s="2"/>
+      <c r="B49" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="18">
-        <f>SUM(C46:C47)</f>
+      <c r="C49" s="18">
+        <f>SUM(C47:C48)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A49" s="163" t="s">
+    <row r="50" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A50" s="163" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="181"/>
-      <c r="C49" s="182"/>
-    </row>
-    <row r="50" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="181"/>
+      <c r="C50" s="182"/>
+    </row>
+    <row r="51" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A51" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C50" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="25"/>
-      <c r="B51" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" s="30">
+      <c r="C51" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="25"/>
-      <c r="B52" s="25" t="s">
-        <v>79</v>
+      <c r="B52" s="29" t="s">
+        <v>66</v>
       </c>
       <c r="C52" s="30">
         <v>0</v>
@@ -16177,624 +16187,629 @@
     </row>
     <row r="53" spans="1:3" ht="13.5" customHeight="1">
       <c r="A53" s="25"/>
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A54" s="25"/>
+      <c r="B54" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C53" s="30">
-        <f>SUM(C50:C52)</f>
+      <c r="C54" s="30">
+        <f>SUM(C51:C53)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="163" t="s">
+    <row r="55" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A55" s="163" t="s">
         <v>22</v>
       </c>
-      <c r="B54" s="181"/>
-      <c r="C54" s="182"/>
-    </row>
-    <row r="55" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A55" s="2" t="s">
+      <c r="B55" s="181"/>
+      <c r="C55" s="182"/>
+    </row>
+    <row r="56" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A56" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="17">
+      <c r="C56" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A56" s="25"/>
-      <c r="B56" s="29" t="s">
+    <row r="57" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A57" s="25"/>
+      <c r="B57" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C56" s="30">
-        <f>SUM(C55)</f>
+      <c r="C57" s="30">
+        <f>SUM(C56)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A57" s="213" t="s">
+    <row r="58" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A58" s="213" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="214"/>
-      <c r="C57" s="215"/>
-    </row>
-    <row r="58" spans="1:3" ht="33" customHeight="1">
-      <c r="A58" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" s="33">
-        <v>0</v>
-      </c>
+      <c r="B58" s="214"/>
+      <c r="C58" s="215"/>
     </row>
     <row r="59" spans="1:3" ht="33" customHeight="1">
       <c r="A59" s="31" t="s">
-        <v>270</v>
+        <v>55</v>
       </c>
       <c r="B59" s="32" t="s">
-        <v>271</v>
+        <v>56</v>
       </c>
       <c r="C59" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="30">
+    <row r="60" spans="1:3" ht="33" customHeight="1">
       <c r="A60" s="31" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C60" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="33" customHeight="1">
+    <row r="61" spans="1:3" ht="30">
       <c r="A61" s="31" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C61" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="19.899999999999999" customHeight="1">
-      <c r="A62" s="31"/>
+    <row r="62" spans="1:3" ht="33" customHeight="1">
+      <c r="A62" s="31" t="s">
+        <v>272</v>
+      </c>
       <c r="B62" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="C62" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A63" s="31"/>
+      <c r="B63" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C62" s="33">
-        <f>SUM(C58:C61)</f>
+      <c r="C63" s="33">
+        <f>SUM(C59:C62)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A63" s="219" t="s">
+    <row r="64" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A64" s="219" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="211"/>
-      <c r="C63" s="193"/>
-    </row>
-    <row r="64" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A64" s="25" t="s">
+      <c r="B64" s="211"/>
+      <c r="C64" s="193"/>
+    </row>
+    <row r="65" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A65" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="25"/>
-      <c r="C64" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="15" customHeight="1">
-      <c r="A65" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" s="27" t="s">
-        <v>64</v>
-      </c>
+      <c r="B65" s="25"/>
       <c r="C65" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A66" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>26</v>
+    <row r="66" spans="1:3" ht="15" customHeight="1">
+      <c r="A66" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" s="27" t="s">
+        <v>64</v>
       </c>
       <c r="C66" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A67" s="31"/>
-      <c r="B67" s="32" t="s">
+      <c r="A67" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A68" s="31"/>
+      <c r="B68" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C67" s="33">
-        <f>SUM(C64:C66)</f>
+      <c r="C68" s="33">
+        <f>SUM(C65:C67)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A68" s="194" t="s">
+    <row r="69" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A69" s="194" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="218"/>
-      <c r="C68" s="196"/>
-    </row>
-    <row r="69" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A69" s="56" t="s">
+      <c r="B69" s="218"/>
+      <c r="C69" s="196"/>
+    </row>
+    <row r="70" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A70" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B69" s="61" t="s">
+      <c r="B70" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="C69" s="58">
+      <c r="C70" s="58">
         <v>330</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A70" s="66" t="s">
+    <row r="71" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A71" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="B70" s="76" t="s">
+      <c r="B71" s="76" t="s">
         <v>111</v>
       </c>
-      <c r="C70" s="67">
+      <c r="C71" s="67">
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="57" t="s">
+    <row r="72" spans="1:3">
+      <c r="A72" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="B71" s="114" t="s">
+      <c r="B72" s="114" t="s">
         <v>349</v>
       </c>
-      <c r="C71" s="59">
+      <c r="C72" s="59">
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A72" s="29" t="s">
+    <row r="73" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A73" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="60" t="s">
+      <c r="B73" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C72" s="30">
+      <c r="C73" s="30">
         <v>900</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A73" s="27"/>
-      <c r="B73" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C73" s="38">
-        <f>SUM(C69:C72)</f>
-        <v>1350</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="13.5" customHeight="1">
       <c r="A74" s="27"/>
-      <c r="B74" s="52" t="s">
+      <c r="B74" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C74" s="38">
+        <f>SUM(C70:C73)</f>
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A75" s="27"/>
+      <c r="B75" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="C74" s="38">
-        <f>C36+C44+C48+C53+C56+C62+C67+C73</f>
+      <c r="C75" s="38">
+        <f>C37+C45+C49+C54+C57+C63+C68+C74</f>
         <v>1577</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A75" s="194" t="s">
+    <row r="76" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A76" s="194" t="s">
         <v>44</v>
       </c>
-      <c r="B75" s="195"/>
-      <c r="C75" s="196"/>
-    </row>
-    <row r="76" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A76" s="41" t="s">
+      <c r="B76" s="195"/>
+      <c r="C76" s="196"/>
+    </row>
+    <row r="77" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A77" s="41" t="s">
         <v>47</v>
-      </c>
-      <c r="B76" s="37"/>
-      <c r="C76" s="123">
-        <f>IF(('July 2024 - September 2024'!C89)+SUM(E90+E97+E107)  &lt; 0,(('July 2024 - September 2024'!C89))+SUM(E90+E97+E107), TEXT((('July 2024 - September 2024'!C89))+SUM(E90+E97+E107),"+$0.00"))</f>
-        <v>-5400</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A77" s="103" t="s">
-        <v>266</v>
       </c>
       <c r="B77" s="37"/>
       <c r="C77" s="123">
+        <f>IF(('July 2024 - September 2024'!C89)+SUM(E91+E98+E108)  &lt; 0,(('July 2024 - September 2024'!C89))+SUM(E91+E98+E108), TEXT((('July 2024 - September 2024'!C89))+SUM(E91+E98+E108),"+$0.00"))</f>
+        <v>-5400</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A78" s="103" t="s">
+        <v>266</v>
+      </c>
+      <c r="B78" s="37"/>
+      <c r="C78" s="123">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A78" s="101" t="s">
+    <row r="79" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A79" s="101" t="s">
         <v>258</v>
       </c>
-      <c r="B78" s="37"/>
-      <c r="C78" s="123" t="str">
-        <f>IF(('July 2024 - September 2024'!C91)+SUM(E89+E98) &lt; 0,(('July 2024 - September 2024'!C91))+SUM(E89+E98), TEXT((('July 2024 - September 2024'!C91))+SUM(E89+E98),"+$0.00"))</f>
+      <c r="B79" s="37"/>
+      <c r="C79" s="123" t="str">
+        <f>IF(('July 2024 - September 2024'!C91)+SUM(E90+E99) &lt; 0,(('July 2024 - September 2024'!C91))+SUM(E90+E99), TEXT((('July 2024 - September 2024'!C91))+SUM(E90+E99),"+$0.00"))</f>
         <v>+$0.00</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="30">
-      <c r="A79" s="63" t="s">
+    <row r="80" spans="1:3" ht="30">
+      <c r="A80" s="63" t="s">
         <v>70</v>
-      </c>
-      <c r="B79" s="53"/>
-      <c r="C79" s="123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="30">
-      <c r="A80" s="77" t="s">
-        <v>112</v>
       </c>
       <c r="B80" s="53"/>
       <c r="C80" s="123">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A81" s="27"/>
-      <c r="B81" s="54" t="s">
+    <row r="81" spans="1:8" ht="30">
+      <c r="A81" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="B81" s="53"/>
+      <c r="C81" s="123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A82" s="27"/>
+      <c r="B82" s="54" t="s">
         <v>358</v>
       </c>
-      <c r="C81" s="48">
-        <f>C76+C77+C78+C79+C80</f>
+      <c r="C82" s="48">
+        <f>C77+C78+C79+C80+C81</f>
         <v>-5400</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A82" s="31"/>
-      <c r="B82" s="39" t="s">
+    <row r="83" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A83" s="31"/>
+      <c r="B83" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C82" s="40">
-        <f>C74</f>
+      <c r="C83" s="40">
+        <f>C75</f>
         <v>1577</v>
       </c>
-      <c r="H82" s="35"/>
-    </row>
-    <row r="83" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A83" s="10"/>
-      <c r="B83" s="10"/>
+      <c r="H83" s="35"/>
     </row>
     <row r="84" spans="1:8" ht="13.5" customHeight="1">
       <c r="A84" s="10"/>
       <c r="B84" s="10"/>
     </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="164" t="s">
+    <row r="85" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A85" s="10"/>
+      <c r="B85" s="10"/>
+    </row>
+    <row r="86" spans="1:8">
+      <c r="A86" s="164" t="s">
         <v>328</v>
       </c>
-      <c r="B85" s="161"/>
-      <c r="C85" s="161"/>
-      <c r="D85" s="161"/>
-      <c r="E85" s="162"/>
-      <c r="G85" s="115" t="s">
+      <c r="B86" s="161"/>
+      <c r="C86" s="161"/>
+      <c r="D86" s="161"/>
+      <c r="E86" s="162"/>
+      <c r="G86" s="115" t="s">
         <v>355</v>
       </c>
-      <c r="H85" s="118">
+      <c r="H86" s="118">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="60">
-      <c r="A86" s="170" t="s">
+    <row r="87" spans="1:8" ht="60">
+      <c r="A87" s="170" t="s">
         <v>38</v>
       </c>
-      <c r="B86" s="215"/>
-      <c r="C86" s="170" t="s">
+      <c r="B87" s="215"/>
+      <c r="C87" s="170" t="s">
         <v>37</v>
       </c>
-      <c r="D86" s="215"/>
-      <c r="E86" s="42" t="s">
+      <c r="D87" s="215"/>
+      <c r="E87" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G86" s="116" t="s">
+      <c r="G87" s="116" t="s">
         <v>356</v>
       </c>
-      <c r="H86" s="117">
-        <f>C69-H85</f>
+      <c r="H87" s="117">
+        <f>C70-H86</f>
         <v>330</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A87" s="189" t="s">
+    <row r="88" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A88" s="189" t="s">
         <v>203</v>
       </c>
-      <c r="B87" s="190"/>
-      <c r="C87" s="178"/>
-      <c r="D87" s="162"/>
-      <c r="E87" s="36">
+      <c r="B88" s="190"/>
+      <c r="C88" s="178"/>
+      <c r="D88" s="162"/>
+      <c r="E88" s="36">
         <f>'July 2024 - September 2024'!E138</f>
         <v>341.01000000000022</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A88" s="152" t="s">
+    <row r="89" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A89" s="152" t="s">
         <v>73</v>
       </c>
-      <c r="B88" s="153"/>
-      <c r="C88" s="165" t="s">
+      <c r="B89" s="153"/>
+      <c r="C89" s="165" t="s">
         <v>351</v>
       </c>
-      <c r="D88" s="237"/>
-      <c r="E88" s="51">
+      <c r="D89" s="237"/>
+      <c r="E89" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A89" s="154"/>
-      <c r="B89" s="155"/>
-      <c r="C89" s="158" t="s">
+    <row r="90" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A90" s="154"/>
+      <c r="B90" s="155"/>
+      <c r="C90" s="158" t="s">
         <v>277</v>
       </c>
-      <c r="D89" s="159"/>
-      <c r="E89" s="51">
+      <c r="D90" s="159"/>
+      <c r="E90" s="51">
         <v>500</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A90" s="156"/>
-      <c r="B90" s="157"/>
-      <c r="C90" s="165" t="s">
+    <row r="91" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A91" s="156"/>
+      <c r="B91" s="157"/>
+      <c r="C91" s="165" t="s">
         <v>281</v>
       </c>
-      <c r="D90" s="165"/>
-      <c r="E90" s="51">
+      <c r="D91" s="165"/>
+      <c r="E91" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A91" s="156" t="s">
+    <row r="92" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A92" s="156" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="157"/>
-      <c r="C91" s="186"/>
-      <c r="D91" s="187"/>
-      <c r="E91" s="43">
-        <f>C82</f>
+      <c r="B92" s="157"/>
+      <c r="C92" s="186"/>
+      <c r="D92" s="187"/>
+      <c r="E92" s="43">
+        <f>C83</f>
         <v>1577</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="13.5" customHeight="1">
-      <c r="C92" s="205" t="s">
+    <row r="93" spans="1:8" ht="13.5" customHeight="1">
+      <c r="C93" s="205" t="s">
         <v>41</v>
       </c>
-      <c r="D92" s="161"/>
-      <c r="E92" s="36">
-        <f>('July 2024 - September 2024'!E138+E13)-SUM(E88:E91)</f>
-        <v>747.01000000000022</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="13.5" customHeight="1"/>
-    <row r="94" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A94" s="164" t="s">
+      <c r="D93" s="161"/>
+      <c r="E93" s="36">
+        <f>('July 2024 - September 2024'!E138+E14)-SUM(E89:E92)</f>
+        <v>921.01000000000022</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="13.5" customHeight="1"/>
+    <row r="95" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A95" s="164" t="s">
         <v>150</v>
       </c>
-      <c r="B94" s="161"/>
-      <c r="C94" s="161"/>
-      <c r="D94" s="161"/>
-      <c r="E94" s="162"/>
-      <c r="G94" s="115" t="s">
+      <c r="B95" s="161"/>
+      <c r="C95" s="161"/>
+      <c r="D95" s="161"/>
+      <c r="E95" s="162"/>
+      <c r="G95" s="115" t="s">
         <v>355</v>
       </c>
-      <c r="H94" s="118">
+      <c r="H95" s="118">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="60">
-      <c r="A95" s="164" t="s">
+    <row r="96" spans="1:8" ht="60">
+      <c r="A96" s="164" t="s">
         <v>38</v>
       </c>
-      <c r="B95" s="162"/>
-      <c r="C95" s="164" t="s">
+      <c r="B96" s="162"/>
+      <c r="C96" s="164" t="s">
         <v>37</v>
       </c>
-      <c r="D95" s="162"/>
-      <c r="E95" s="22" t="s">
+      <c r="D96" s="162"/>
+      <c r="E96" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G95" s="116" t="s">
+      <c r="G96" s="116" t="s">
         <v>356</v>
       </c>
-      <c r="H95" s="117">
-        <f>C69-H94</f>
+      <c r="H96" s="117">
+        <f>C70-H95</f>
         <v>330</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A96" s="201" t="s">
+    <row r="97" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A97" s="201" t="s">
         <v>87</v>
       </c>
-      <c r="B96" s="225"/>
-      <c r="C96" s="258"/>
-      <c r="D96" s="259"/>
-      <c r="E96" s="36">
-        <f>E92</f>
-        <v>747.01000000000022</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A97" s="189" t="s">
+      <c r="B97" s="225"/>
+      <c r="C97" s="258"/>
+      <c r="D97" s="259"/>
+      <c r="E97" s="36">
+        <f>E93</f>
+        <v>921.01000000000022</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A98" s="189" t="s">
         <v>73</v>
       </c>
-      <c r="B97" s="254"/>
-      <c r="C97" s="183" t="s">
+      <c r="B98" s="254"/>
+      <c r="C98" s="183" t="s">
         <v>367</v>
       </c>
-      <c r="D97" s="257"/>
-      <c r="E97" s="51">
+      <c r="D98" s="257"/>
+      <c r="E98" s="51">
         <v>700</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A98" s="255"/>
-      <c r="B98" s="256"/>
-      <c r="C98" s="183" t="s">
+    <row r="99" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A99" s="255"/>
+      <c r="B99" s="256"/>
+      <c r="C99" s="183" t="s">
         <v>368</v>
       </c>
-      <c r="D98" s="177"/>
-      <c r="E98" s="51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A99" s="197"/>
-      <c r="B99" s="200"/>
-      <c r="C99" s="183" t="s">
-        <v>364</v>
-      </c>
-      <c r="D99" s="176"/>
+      <c r="D99" s="177"/>
       <c r="E99" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A100" s="201" t="s">
+      <c r="A100" s="197"/>
+      <c r="B100" s="200"/>
+      <c r="C100" s="183" t="s">
+        <v>364</v>
+      </c>
+      <c r="D100" s="176"/>
+      <c r="E100" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A101" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="B100" s="225"/>
-      <c r="C100" s="178"/>
-      <c r="D100" s="162"/>
-      <c r="E100" s="64">
-        <f>C82</f>
+      <c r="B101" s="225"/>
+      <c r="C101" s="178"/>
+      <c r="D101" s="162"/>
+      <c r="E101" s="64">
+        <f>C83</f>
         <v>1577</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="13.5" customHeight="1">
-      <c r="C101" s="188" t="s">
+    <row r="102" spans="1:8" ht="13.5" customHeight="1">
+      <c r="C102" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="D101" s="162"/>
-      <c r="E101" s="36">
-        <f>(E19+E96)-SUM(E97:E100)</f>
-        <v>875.01000000000022</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A102" s="23"/>
-      <c r="B102" s="23"/>
-      <c r="C102" s="23"/>
-      <c r="D102" s="23"/>
-      <c r="E102" s="23"/>
-    </row>
-    <row r="103" spans="1:8" ht="17.25" customHeight="1">
+      <c r="D102" s="162"/>
+      <c r="E102" s="36">
+        <f>(E20+E97)-SUM(E98:E101)</f>
+        <v>1049.0100000000002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="13.5" customHeight="1">
       <c r="A103" s="23"/>
       <c r="B103" s="23"/>
       <c r="C103" s="23"/>
       <c r="D103" s="23"/>
       <c r="E103" s="23"/>
     </row>
-    <row r="104" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A104" s="191" t="s">
+    <row r="104" spans="1:8" ht="17.25" customHeight="1">
+      <c r="A104" s="23"/>
+      <c r="B104" s="23"/>
+      <c r="C104" s="23"/>
+      <c r="D104" s="23"/>
+      <c r="E104" s="23"/>
+    </row>
+    <row r="105" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A105" s="191" t="s">
         <v>151</v>
       </c>
-      <c r="B104" s="192"/>
-      <c r="C104" s="192"/>
-      <c r="D104" s="192"/>
-      <c r="E104" s="193"/>
-      <c r="G104" s="115" t="s">
+      <c r="B105" s="192"/>
+      <c r="C105" s="192"/>
+      <c r="D105" s="192"/>
+      <c r="E105" s="193"/>
+      <c r="G105" s="115" t="s">
         <v>355</v>
       </c>
-      <c r="H104" s="118">
+      <c r="H105" s="118">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="60">
-      <c r="A105" s="164" t="s">
+    <row r="106" spans="1:8" ht="60">
+      <c r="A106" s="164" t="s">
         <v>38</v>
       </c>
-      <c r="B105" s="162"/>
-      <c r="C105" s="164" t="s">
+      <c r="B106" s="162"/>
+      <c r="C106" s="164" t="s">
         <v>37</v>
       </c>
-      <c r="D105" s="162"/>
-      <c r="E105" s="22" t="s">
+      <c r="D106" s="162"/>
+      <c r="E106" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G105" s="116" t="s">
+      <c r="G106" s="116" t="s">
         <v>356</v>
       </c>
-      <c r="H105" s="117">
-        <f>C69-H104</f>
+      <c r="H106" s="117">
+        <f>C70-H105</f>
         <v>330</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A106" s="201" t="s">
+    <row r="107" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A107" s="201" t="s">
         <v>90</v>
       </c>
-      <c r="B106" s="225"/>
-      <c r="C106" s="178"/>
-      <c r="D106" s="162"/>
-      <c r="E106" s="36">
-        <f>E101</f>
-        <v>875.01000000000022</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A107" s="189" t="s">
+      <c r="B107" s="225"/>
+      <c r="C107" s="178"/>
+      <c r="D107" s="162"/>
+      <c r="E107" s="36">
+        <f>E102</f>
+        <v>1049.0100000000002</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A108" s="189" t="s">
         <v>73</v>
       </c>
-      <c r="B107" s="254"/>
-      <c r="C107" s="183" t="s">
+      <c r="B108" s="254"/>
+      <c r="C108" s="183" t="s">
         <v>365</v>
       </c>
-      <c r="D107" s="184"/>
-      <c r="E107" s="51">
+      <c r="D108" s="184"/>
+      <c r="E108" s="51">
         <v>800</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A108" s="197"/>
-      <c r="B108" s="200"/>
-      <c r="C108" s="183" t="s">
+    <row r="109" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A109" s="197"/>
+      <c r="B109" s="200"/>
+      <c r="C109" s="183" t="s">
         <v>357</v>
       </c>
-      <c r="D108" s="176"/>
-      <c r="E108" s="51">
+      <c r="D109" s="176"/>
+      <c r="E109" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A109" s="201" t="s">
+    <row r="110" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A110" s="201" t="s">
         <v>40</v>
       </c>
-      <c r="B109" s="225"/>
-      <c r="C109" s="178"/>
-      <c r="D109" s="162"/>
-      <c r="E109" s="64">
-        <f>C82</f>
+      <c r="B110" s="225"/>
+      <c r="C110" s="178"/>
+      <c r="D110" s="162"/>
+      <c r="E110" s="64">
+        <f>C83</f>
         <v>1577</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="13.5" customHeight="1">
-      <c r="C110" s="188" t="s">
+    <row r="111" spans="1:8" ht="13.5" customHeight="1">
+      <c r="C111" s="188" t="s">
         <v>28</v>
       </c>
-      <c r="D110" s="162"/>
-      <c r="E110" s="51">
-        <f>(E25+E106)-SUM(E107:E109)</f>
-        <v>903.01000000000022</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A111" s="10"/>
-      <c r="B111" s="10"/>
+      <c r="D111" s="162"/>
+      <c r="E111" s="51">
+        <f>(E26+E107)-SUM(E108:E110)</f>
+        <v>1077.0100000000002</v>
+      </c>
     </row>
     <row r="112" spans="1:8" ht="13.5" customHeight="1">
       <c r="A112" s="10"/>
@@ -20444,67 +20459,72 @@
       <c r="A1023" s="10"/>
       <c r="B1023" s="10"/>
     </row>
+    <row r="1024" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A1024" s="10"/>
+      <c r="B1024" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="60">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="A86:E86"/>
     <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A85:E85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="A107:B108"/>
+    <mergeCell ref="A108:B109"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C89:D89"/>
     <mergeCell ref="C108:D108"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A95:E95"/>
+    <mergeCell ref="A96:B96"/>
     <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="A107:B107"/>
     <mergeCell ref="C107:D107"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A94:E94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C102:D102"/>
     <mergeCell ref="A106:B106"/>
     <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A98:B100"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="A101:B101"/>
     <mergeCell ref="C101:D101"/>
-    <mergeCell ref="A104:E104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A97:B99"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="A100:B100"/>
     <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="A37:C38"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A88:B90"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A89:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A105:E105"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="106" priority="9" operator="lessThan">
@@ -20519,7 +20539,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76:C80">
+  <conditionalFormatting sqref="C77:C81">
     <cfRule type="cellIs" dxfId="103" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -20527,7 +20547,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="E88">
     <cfRule type="cellIs" dxfId="101" priority="6" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20535,7 +20555,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
+  <conditionalFormatting sqref="E93">
     <cfRule type="cellIs" dxfId="99" priority="18" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20543,7 +20563,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E96">
+  <conditionalFormatting sqref="E97">
     <cfRule type="cellIs" dxfId="97" priority="14" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20551,7 +20571,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E101">
+  <conditionalFormatting sqref="E102">
     <cfRule type="cellIs" dxfId="95" priority="16" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20559,7 +20579,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E106">
+  <conditionalFormatting sqref="E107">
     <cfRule type="cellIs" dxfId="93" priority="12" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20567,7 +20587,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E110">
+  <conditionalFormatting sqref="E111">
     <cfRule type="cellIs" dxfId="91" priority="10" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20630,7 +20650,7 @@
       </c>
       <c r="C3" s="4">
         <f>E106</f>
-        <v>987.01000000000022</v>
+        <v>1161.0100000000002</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -20662,7 +20682,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>987.01000000000022</v>
+        <v>1161.0100000000002</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -21476,7 +21496,7 @@
       </c>
       <c r="B75" s="37"/>
       <c r="C75" s="123">
-        <f>IF(('October 2024 - December 2024'!C76)+SUM(E86+E95+E103)  &lt; 0,(('October 2024 - December 2024'!C76))+SUM(E86+E95+E103), TEXT((('October 2024 - December 2024'!C76))+SUM(E86+E95+E103),"+$0.00"))</f>
+        <f>IF(('October 2024 - December 2024'!C77)+SUM(E86+E95+E103)  &lt; 0,(('October 2024 - December 2024'!C77))+SUM(E86+E95+E103), TEXT((('October 2024 - December 2024'!C77))+SUM(E86+E95+E103),"+$0.00"))</f>
         <v>-3000</v>
       </c>
     </row>
@@ -21495,7 +21515,7 @@
       </c>
       <c r="B77" s="37"/>
       <c r="C77" s="123" t="str">
-        <f>IF(('October 2024 - December 2024'!C78)+SUM(0) &lt; 0,(('October 2024 - December 2024'!C78))+SUM(0), TEXT((('October 2024 - December 2024'!C78))+SUM(0),"+$0.00"))</f>
+        <f>IF(('October 2024 - December 2024'!C79)+SUM(0) &lt; 0,(('October 2024 - December 2024'!C79))+SUM(0), TEXT((('October 2024 - December 2024'!C79))+SUM(0),"+$0.00"))</f>
         <v>+$0.00</v>
       </c>
     </row>
@@ -21623,8 +21643,8 @@
       </c>
       <c r="D89" s="211"/>
       <c r="E89" s="36">
-        <f>('October 2024 - December 2024'!E110+E12)-SUM(E86:E88)</f>
-        <v>931.01000000000022</v>
+        <f>('October 2024 - December 2024'!E111+E12)-SUM(E86:E88)</f>
+        <v>1105.0100000000002</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="13.5" customHeight="1"/>
@@ -21672,7 +21692,7 @@
       <c r="D93" s="259"/>
       <c r="E93" s="36">
         <f>E89</f>
-        <v>931.01000000000022</v>
+        <v>1105.0100000000002</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1">
@@ -21718,7 +21738,7 @@
       <c r="D97" s="162"/>
       <c r="E97" s="36">
         <f>(E18+E93)-SUM(E94:E96)</f>
-        <v>959.01000000000022</v>
+        <v>1133.0100000000002</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="13.5" customHeight="1">
@@ -21779,7 +21799,7 @@
       <c r="D102" s="162"/>
       <c r="E102" s="36">
         <f>E97</f>
-        <v>959.01000000000022</v>
+        <v>1133.0100000000002</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" customHeight="1">
@@ -21825,7 +21845,7 @@
       <c r="D106" s="193"/>
       <c r="E106" s="100">
         <f>(E24+E102)-SUM(E103:E105)</f>
-        <v>987.01000000000022</v>
+        <v>1161.0100000000002</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">
@@ -25653,7 +25673,7 @@
       </c>
       <c r="C3" s="4">
         <f>E106</f>
-        <v>471.01000000000022</v>
+        <v>645.01000000000022</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -25685,7 +25705,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>471.01000000000022</v>
+        <v>645.01000000000022</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -26650,7 +26670,7 @@
       <c r="D89" s="211"/>
       <c r="E89" s="73">
         <f>('January 2025 - March 2025'!E106+E12)-SUM(E86:E88)</f>
-        <v>815.01000000000022</v>
+        <v>989.01000000000022</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="13.5" customHeight="1"/>
@@ -26698,7 +26718,7 @@
       <c r="D93" s="259"/>
       <c r="E93" s="36">
         <f>E89</f>
-        <v>815.01000000000022</v>
+        <v>989.01000000000022</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1">
@@ -26744,7 +26764,7 @@
       <c r="D97" s="162"/>
       <c r="E97" s="36">
         <f>(E18+E93)-SUM(E94:E96)</f>
-        <v>643.01000000000022</v>
+        <v>817.01000000000022</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="13.5" customHeight="1">
@@ -26805,7 +26825,7 @@
       <c r="D102" s="162"/>
       <c r="E102" s="36">
         <f>E97</f>
-        <v>643.01000000000022</v>
+        <v>817.01000000000022</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" customHeight="1">
@@ -26851,7 +26871,7 @@
       <c r="D106" s="162"/>
       <c r="E106" s="51">
         <f>(E24+E102)-SUM(E103:E105)</f>
-        <v>471.01000000000022</v>
+        <v>645.01000000000022</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">
@@ -30681,7 +30701,7 @@
       </c>
       <c r="C3" s="4">
         <f>E106</f>
-        <v>2955.01</v>
+        <v>3129.01</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -30713,7 +30733,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>2955.01</v>
+        <v>3129.01</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -31677,7 +31697,7 @@
       <c r="D89" s="211"/>
       <c r="E89" s="73">
         <f>('April 2025 - June 2025'!E106+E12)-SUM(E86:E88)</f>
-        <v>1299.0100000000002</v>
+        <v>1473.0100000000002</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="13.5" customHeight="1"/>
@@ -31725,7 +31745,7 @@
       <c r="D93" s="239"/>
       <c r="E93" s="86">
         <f>E89</f>
-        <v>1299.0100000000002</v>
+        <v>1473.0100000000002</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1">
@@ -31771,7 +31791,7 @@
       <c r="D97" s="193"/>
       <c r="E97" s="73">
         <f>(E18+E93)-SUM(E94:E96)</f>
-        <v>2127.0100000000002</v>
+        <v>2301.0100000000002</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="13.5" customHeight="1">
@@ -31832,7 +31852,7 @@
       <c r="D102" s="261"/>
       <c r="E102" s="36">
         <f>E97</f>
-        <v>2127.0100000000002</v>
+        <v>2301.0100000000002</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" customHeight="1">
@@ -31878,7 +31898,7 @@
       <c r="D106" s="193"/>
       <c r="E106" s="100">
         <f>(E24+E102)-SUM(E103:E105)</f>
-        <v>2955.01</v>
+        <v>3129.01</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">
@@ -35709,7 +35729,7 @@
       </c>
       <c r="C3" s="4">
         <f>E106</f>
-        <v>5439.01</v>
+        <v>5613.01</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -35741,7 +35761,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>5439.01</v>
+        <v>5613.01</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -36705,7 +36725,7 @@
       <c r="D89" s="211"/>
       <c r="E89" s="73">
         <f>('July 2025 - September 2025'!E106+E12)-SUM(E86:E88)</f>
-        <v>3783.01</v>
+        <v>3957.01</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="13.5" customHeight="1"/>
@@ -36753,7 +36773,7 @@
       <c r="D93" s="259"/>
       <c r="E93" s="36">
         <f>E89</f>
-        <v>3783.01</v>
+        <v>3957.01</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1">
@@ -36799,7 +36819,7 @@
       <c r="D97" s="162"/>
       <c r="E97" s="36">
         <f>(E18+E93)-SUM(E94:E96)</f>
-        <v>4611.01</v>
+        <v>4785.01</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="13.5" customHeight="1">
@@ -36860,7 +36880,7 @@
       <c r="D102" s="162"/>
       <c r="E102" s="36">
         <f>E97</f>
-        <v>4611.01</v>
+        <v>4785.01</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" customHeight="1">
@@ -36906,7 +36926,7 @@
       <c r="D106" s="162"/>
       <c r="E106" s="51">
         <f>(E24+E102)-SUM(E103:E105)</f>
-        <v>5439.01</v>
+        <v>5613.01</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">
@@ -40738,7 +40758,7 @@
       </c>
       <c r="C3" s="4">
         <f>E106</f>
-        <v>7923.01</v>
+        <v>8097.01</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -40770,7 +40790,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>7923.01</v>
+        <v>8097.01</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -41734,7 +41754,7 @@
       <c r="D89" s="211"/>
       <c r="E89" s="73">
         <f>('October 2025 - December 2025'!E106+E12)-SUM(E86:E88)</f>
-        <v>6267.01</v>
+        <v>6441.01</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="13.5" customHeight="1"/>
@@ -41782,7 +41802,7 @@
       <c r="D93" s="259"/>
       <c r="E93" s="36">
         <f>E89</f>
-        <v>6267.01</v>
+        <v>6441.01</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1">
@@ -41828,7 +41848,7 @@
       <c r="D97" s="162"/>
       <c r="E97" s="36">
         <f>(E18+E93)-SUM(E94:E96)</f>
-        <v>7095.01</v>
+        <v>7269.01</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="13.5" customHeight="1">
@@ -41889,7 +41909,7 @@
       <c r="D102" s="162"/>
       <c r="E102" s="36">
         <f>E97</f>
-        <v>7095.01</v>
+        <v>7269.01</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" customHeight="1">
@@ -41935,7 +41955,7 @@
       <c r="D106" s="162"/>
       <c r="E106" s="51">
         <f>(E24+E102)-SUM(E103:E105)</f>
-        <v>7923.01</v>
+        <v>8097.01</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">
@@ -45767,7 +45787,7 @@
       </c>
       <c r="C3" s="4">
         <f>E106</f>
-        <v>10407.01</v>
+        <v>10581.01</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -45799,7 +45819,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>10407.01</v>
+        <v>10581.01</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -46763,7 +46783,7 @@
       <c r="D89" s="211"/>
       <c r="E89" s="73">
         <f>('January 2026 - March 2026'!E106+E12)-SUM(E86:E88)</f>
-        <v>8751.01</v>
+        <v>8925.01</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="13.5" customHeight="1"/>
@@ -46811,7 +46831,7 @@
       <c r="D93" s="259"/>
       <c r="E93" s="36">
         <f>E89</f>
-        <v>8751.01</v>
+        <v>8925.01</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1">
@@ -46857,7 +46877,7 @@
       <c r="D97" s="162"/>
       <c r="E97" s="36">
         <f>(E18+E93)-SUM(E94:E96)</f>
-        <v>9579.01</v>
+        <v>9753.01</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="13.5" customHeight="1">
@@ -46918,7 +46938,7 @@
       <c r="D102" s="162"/>
       <c r="E102" s="36">
         <f>E97</f>
-        <v>9579.01</v>
+        <v>9753.01</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" customHeight="1">
@@ -46964,7 +46984,7 @@
       <c r="D106" s="162"/>
       <c r="E106" s="51">
         <f>(E24+E102)-SUM(E103:E105)</f>
-        <v>10407.01</v>
+        <v>10581.01</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">

</xml_diff>

<commit_message>
docs: Income and Expense Updated.
</commit_message>
<xml_diff>
--- a/Alan Tang_s Income Expense Future.xlsx
+++ b/Alan Tang_s Income Expense Future.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Income-Expenditure-Forecast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEA3EA0-D819-46F5-9A02-467C03418C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D091B5-B942-4EB7-8313-47DBF3278556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="April 2024 - June 2024" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="414">
   <si>
     <t>Assets</t>
   </si>
@@ -1419,6 +1419,12 @@
   </si>
   <si>
     <t>4. Additional China Mobile Fee For Joox Refund $207 - $149</t>
+  </si>
+  <si>
+    <t>19th October 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Octopus AddIn Value $50 </t>
   </si>
 </sst>
 </file>
@@ -2994,9 +3000,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="29" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3051,11 +3054,11 @@
     <xf numFmtId="166" fontId="27" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="27" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3066,6 +3069,12 @@
     <xf numFmtId="166" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3075,17 +3084,14 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4309,7 +4315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1053"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -4368,7 +4374,7 @@
         <v>78</v>
       </c>
       <c r="C3" s="4">
-        <v>2347.61</v>
+        <v>1247.6099999999999</v>
       </c>
       <c r="D3" s="90" t="s">
         <v>0</v>
@@ -4377,7 +4383,7 @@
         <v>78</v>
       </c>
       <c r="F3" s="91">
-        <v>175.61</v>
+        <v>2347.61</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="94" t="s">
@@ -4609,22 +4615,22 @@
         <v>130</v>
       </c>
       <c r="C9" s="4">
-        <v>28</v>
+        <v>178</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="34" t="s">
         <v>130</v>
       </c>
       <c r="F9" s="4">
-        <v>96</v>
+        <v>28</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="94" t="s">
         <v>307</v>
       </c>
       <c r="I9" s="95">
-        <f>'October 2024 - December 2024'!E98</f>
-        <v>1300.71</v>
+        <f>'October 2024 - December 2024'!E99</f>
+        <v>1350.71</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -4649,22 +4655,22 @@
         <v>48</v>
       </c>
       <c r="C10" s="4">
-        <v>14.4</v>
+        <v>12.4</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="34" t="s">
         <v>48</v>
       </c>
       <c r="F10" s="55">
-        <v>12.4</v>
+        <v>14.4</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="94" t="s">
         <v>170</v>
       </c>
       <c r="I10" s="95">
-        <f>'October 2024 - December 2024'!E107</f>
-        <v>2386.71</v>
+        <f>'October 2024 - December 2024'!E108</f>
+        <v>2436.71</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -4690,7 +4696,7 @@
       </c>
       <c r="C11" s="4">
         <f>SUM(C3:C10)</f>
-        <v>2408.71</v>
+        <v>1456.71</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="62" t="s">
@@ -4698,15 +4704,15 @@
       </c>
       <c r="F11" s="55">
         <f>SUM(F3:F10)</f>
-        <v>302.70999999999998</v>
+        <v>2408.71</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="94" t="s">
         <v>171</v>
       </c>
       <c r="I11" s="95">
-        <f>'October 2024 - December 2024'!E116</f>
-        <v>3322.71</v>
+        <f>'October 2024 - December 2024'!E117</f>
+        <v>3372.71</v>
       </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -4743,7 +4749,7 @@
       </c>
       <c r="I12" s="95">
         <f>'January 2025 - March 2025'!E93</f>
-        <v>3005.71</v>
+        <v>3055.71</v>
       </c>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -4775,7 +4781,7 @@
       </c>
       <c r="I13" s="95">
         <f>'January 2025 - March 2025'!E101</f>
-        <v>823.86999999999989</v>
+        <v>873.86999999999989</v>
       </c>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
@@ -4800,7 +4806,7 @@
       </c>
       <c r="I14" s="95">
         <f>'January 2025 - March 2025'!E110</f>
-        <v>841.86999999999989</v>
+        <v>891.86999999999989</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="30" customHeight="1">
@@ -4817,7 +4823,7 @@
       </c>
       <c r="I15" s="95">
         <f>'April 2025 - June 2025'!E92</f>
-        <v>927.86999999999989</v>
+        <v>977.86999999999989</v>
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
@@ -4855,7 +4861,7 @@
       </c>
       <c r="I16" s="95">
         <f>'April 2025 - June 2025'!E100</f>
-        <v>1081.8699999999999</v>
+        <v>1131.8699999999999</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="30" customHeight="1">
@@ -4877,7 +4883,7 @@
       </c>
       <c r="I17" s="95">
         <f>'April 2025 - June 2025'!E109</f>
-        <v>1099.8699999999999</v>
+        <v>1149.8699999999999</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="30" customHeight="1">
@@ -4896,7 +4902,7 @@
       </c>
       <c r="I18" s="95">
         <f>'July 2025 - September 2025'!E92</f>
-        <v>803.86999999999989</v>
+        <v>853.86999999999989</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="30" customHeight="1">
@@ -4907,7 +4913,7 @@
       </c>
       <c r="I19" s="95">
         <f>'July 2025 - September 2025'!E100</f>
-        <v>389.86999999999989</v>
+        <v>439.86999999999989</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="30" customHeight="1">
@@ -4924,7 +4930,7 @@
       </c>
       <c r="I20" s="95">
         <f>'July 2025 - September 2025'!E109</f>
-        <v>1407.87</v>
+        <v>1457.87</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
@@ -4963,7 +4969,7 @@
       </c>
       <c r="I21" s="95">
         <f>'October 2025 - December 2025'!E93</f>
-        <v>2493.87</v>
+        <v>2543.87</v>
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
@@ -5002,7 +5008,7 @@
       </c>
       <c r="I22" s="95">
         <f>'October 2025 - December 2025'!E101</f>
-        <v>3497.87</v>
+        <v>3547.87</v>
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
@@ -5041,7 +5047,7 @@
       </c>
       <c r="I23" s="129">
         <f>'October 2025 - December 2025'!E110</f>
-        <v>4583.87</v>
+        <v>4633.87</v>
       </c>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
@@ -5094,7 +5100,7 @@
       </c>
       <c r="I25" s="95">
         <f>'January 2026 - March 2026'!E92</f>
-        <v>5519.87</v>
+        <v>5569.87</v>
       </c>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
@@ -5125,7 +5131,7 @@
       </c>
       <c r="I26" s="95">
         <f>'January 2026 - March 2026'!E100</f>
-        <v>6605.87</v>
+        <v>6655.87</v>
       </c>
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
@@ -5156,7 +5162,7 @@
       </c>
       <c r="I27" s="95">
         <f>'January 2026 - March 2026'!E109</f>
-        <v>7691.869999999999</v>
+        <v>7741.869999999999</v>
       </c>
       <c r="J27" s="13"/>
       <c r="K27" s="13"/>
@@ -5189,7 +5195,7 @@
       </c>
       <c r="I28" s="95">
         <f>'April 2026 - June 2026'!E92</f>
-        <v>8627.869999999999</v>
+        <v>8677.869999999999</v>
       </c>
       <c r="J28" s="13"/>
       <c r="K28" s="13"/>
@@ -5228,7 +5234,7 @@
       </c>
       <c r="I29" s="151">
         <f>'April 2026 - June 2026'!E100</f>
-        <v>9713.869999999999</v>
+        <v>9763.869999999999</v>
       </c>
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
@@ -5293,7 +5299,7 @@
       </c>
       <c r="I32" s="95">
         <f>'April 2026 - June 2026'!E109</f>
-        <v>10799.869999999999</v>
+        <v>10849.869999999999</v>
       </c>
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
@@ -10257,8 +10263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5F3FA5-5013-4B35-A74B-6269617B858B}">
   <dimension ref="A1:Y1055"/>
   <sheetViews>
-    <sheetView topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E138" sqref="E138"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -10456,7 +10462,7 @@
       <c r="B9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="250" t="s">
+      <c r="C9" s="249" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="219"/>
@@ -10565,7 +10571,7 @@
       <c r="B17" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="250" t="s">
+      <c r="C17" s="249" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="219"/>
@@ -10580,7 +10586,7 @@
       <c r="B18" s="31" t="s">
         <v>250</v>
       </c>
-      <c r="C18" s="255" t="s">
+      <c r="C18" s="254" t="s">
         <v>283</v>
       </c>
       <c r="D18" s="226"/>
@@ -10595,7 +10601,7 @@
       <c r="B19" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="C19" s="255" t="s">
+      <c r="C19" s="254" t="s">
         <v>284</v>
       </c>
       <c r="D19" s="226"/>
@@ -10610,7 +10616,7 @@
       <c r="B20" s="31" t="s">
         <v>254</v>
       </c>
-      <c r="C20" s="255" t="s">
+      <c r="C20" s="254" t="s">
         <v>285</v>
       </c>
       <c r="D20" s="226"/>
@@ -10739,7 +10745,7 @@
       <c r="B29" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C29" s="250" t="s">
+      <c r="C29" s="249" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="219"/>
@@ -10757,7 +10763,7 @@
       <c r="C30" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="251"/>
+      <c r="D30" s="250"/>
       <c r="E30" s="65">
         <v>0</v>
       </c>
@@ -10921,7 +10927,7 @@
       <c r="B44" s="10"/>
     </row>
     <row r="45" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A45" s="249" t="s">
+      <c r="A45" s="248" t="s">
         <v>85</v>
       </c>
       <c r="B45" s="165"/>
@@ -11458,7 +11464,7 @@
       <c r="C102" s="169" t="s">
         <v>200</v>
       </c>
-      <c r="D102" s="252"/>
+      <c r="D102" s="251"/>
       <c r="E102" s="51">
         <v>1000</v>
       </c>
@@ -11565,10 +11571,10 @@
     <row r="112" spans="1:8" ht="13.5" customHeight="1">
       <c r="A112" s="160"/>
       <c r="B112" s="161"/>
-      <c r="C112" s="246" t="s">
+      <c r="C112" s="245" t="s">
         <v>282</v>
       </c>
-      <c r="D112" s="247"/>
+      <c r="D112" s="246"/>
       <c r="E112" s="51">
         <v>139.28</v>
       </c>
@@ -11578,15 +11584,15 @@
         <v>40</v>
       </c>
       <c r="B113" s="161"/>
-      <c r="C113" s="245"/>
-      <c r="D113" s="245"/>
+      <c r="C113" s="244"/>
+      <c r="D113" s="244"/>
       <c r="E113" s="74">
         <f>C97</f>
         <v>2028.5</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C114" s="248" t="s">
+      <c r="C114" s="247" t="s">
         <v>41</v>
       </c>
       <c r="D114" s="215"/>
@@ -11623,8 +11629,8 @@
         <v>72</v>
       </c>
       <c r="B118" s="194"/>
-      <c r="C118" s="243"/>
-      <c r="D118" s="244"/>
+      <c r="C118" s="242"/>
+      <c r="D118" s="243"/>
       <c r="E118" s="86">
         <f>E114</f>
         <v>499.83999999999924</v>
@@ -11635,10 +11641,10 @@
         <v>73</v>
       </c>
       <c r="B119" s="157"/>
-      <c r="C119" s="253" t="s">
+      <c r="C119" s="252" t="s">
         <v>252</v>
       </c>
-      <c r="D119" s="254"/>
+      <c r="D119" s="253"/>
       <c r="E119" s="87">
         <v>72</v>
       </c>
@@ -11646,10 +11652,10 @@
     <row r="120" spans="1:5" ht="13.5" customHeight="1">
       <c r="A120" s="158"/>
       <c r="B120" s="159"/>
-      <c r="C120" s="253" t="s">
+      <c r="C120" s="252" t="s">
         <v>253</v>
       </c>
-      <c r="D120" s="254"/>
+      <c r="D120" s="253"/>
       <c r="E120" s="87">
         <v>55.3</v>
       </c>
@@ -11660,7 +11666,7 @@
       <c r="C121" s="169" t="s">
         <v>269</v>
       </c>
-      <c r="D121" s="252"/>
+      <c r="D121" s="251"/>
       <c r="E121" s="84">
         <v>0</v>
       </c>
@@ -11701,10 +11707,10 @@
     <row r="125" spans="1:5" ht="13.5" customHeight="1">
       <c r="A125" s="160"/>
       <c r="B125" s="161"/>
-      <c r="C125" s="246" t="s">
+      <c r="C125" s="245" t="s">
         <v>287</v>
       </c>
-      <c r="D125" s="247"/>
+      <c r="D125" s="246"/>
       <c r="E125" s="51">
         <v>464.47</v>
       </c>
@@ -11714,7 +11720,7 @@
         <v>40</v>
       </c>
       <c r="B126" s="202"/>
-      <c r="C126" s="257"/>
+      <c r="C126" s="256"/>
       <c r="D126" s="197"/>
       <c r="E126" s="64">
         <f>C97</f>
@@ -11793,21 +11799,21 @@
       </c>
     </row>
     <row r="133" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A133" s="241" t="s">
+      <c r="A133" s="259" t="s">
         <v>73</v>
       </c>
-      <c r="B133" s="241"/>
+      <c r="B133" s="259"/>
       <c r="C133" s="172" t="s">
         <v>324</v>
       </c>
-      <c r="D133" s="256"/>
+      <c r="D133" s="255"/>
       <c r="E133" s="71">
         <v>130.84</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A134" s="241"/>
-      <c r="B134" s="241"/>
+      <c r="A134" s="259"/>
+      <c r="B134" s="259"/>
       <c r="C134" s="208" t="s">
         <v>313</v>
       </c>
@@ -11817,8 +11823,8 @@
       </c>
     </row>
     <row r="135" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A135" s="241"/>
-      <c r="B135" s="241"/>
+      <c r="A135" s="259"/>
+      <c r="B135" s="259"/>
       <c r="C135" s="208" t="s">
         <v>270</v>
       </c>
@@ -11828,8 +11834,8 @@
       </c>
     </row>
     <row r="136" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A136" s="241"/>
-      <c r="B136" s="241"/>
+      <c r="A136" s="259"/>
+      <c r="B136" s="259"/>
       <c r="C136" s="208" t="s">
         <v>289</v>
       </c>
@@ -11839,8 +11845,8 @@
       </c>
     </row>
     <row r="137" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A137" s="241"/>
-      <c r="B137" s="241"/>
+      <c r="A137" s="259"/>
+      <c r="B137" s="259"/>
       <c r="C137" s="208" t="s">
         <v>323</v>
       </c>
@@ -11850,9 +11856,9 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="147" customHeight="1">
-      <c r="A138" s="241"/>
-      <c r="B138" s="241"/>
-      <c r="C138" s="258" t="s">
+      <c r="A138" s="259"/>
+      <c r="B138" s="259"/>
+      <c r="C138" s="257" t="s">
         <v>409</v>
       </c>
       <c r="D138" s="169"/>
@@ -11861,23 +11867,23 @@
       </c>
     </row>
     <row r="139" spans="1:8" ht="21" customHeight="1">
-      <c r="A139" s="241"/>
-      <c r="B139" s="241"/>
-      <c r="C139" s="259" t="s">
+      <c r="A139" s="259"/>
+      <c r="B139" s="259"/>
+      <c r="C139" s="258" t="s">
         <v>246</v>
       </c>
-      <c r="D139" s="258"/>
+      <c r="D139" s="257"/>
       <c r="E139" s="100">
         <v>600</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A140" s="241"/>
-      <c r="B140" s="241"/>
-      <c r="C140" s="242" t="s">
+      <c r="A140" s="259"/>
+      <c r="B140" s="259"/>
+      <c r="C140" s="241" t="s">
         <v>408</v>
       </c>
-      <c r="D140" s="242"/>
+      <c r="D140" s="241"/>
       <c r="E140" s="100">
         <v>9.5</v>
       </c>
@@ -11887,7 +11893,7 @@
         <v>40</v>
       </c>
       <c r="B141" s="202"/>
-      <c r="C141" s="257"/>
+      <c r="C141" s="256"/>
       <c r="D141" s="215"/>
       <c r="E141" s="107">
         <f>C97</f>
@@ -15581,16 +15587,13 @@
     <mergeCell ref="C138:D138"/>
     <mergeCell ref="C139:D139"/>
     <mergeCell ref="C137:D137"/>
+    <mergeCell ref="A133:B140"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="A119:B125"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="A118:B118"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="C38:D38"/>
@@ -15598,13 +15601,16 @@
     <mergeCell ref="C111:D111"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="A102:B112"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="A119:B125"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="A118:B118"/>
     <mergeCell ref="C121:D121"/>
     <mergeCell ref="C119:D119"/>
     <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="A116:E116"/>
-    <mergeCell ref="A117:B117"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="C103:D103"/>
@@ -15632,7 +15638,6 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C31:D31"/>
-    <mergeCell ref="A133:B140"/>
     <mergeCell ref="C140:D140"/>
     <mergeCell ref="C118:D118"/>
     <mergeCell ref="C105:D105"/>
@@ -15642,12 +15647,13 @@
     <mergeCell ref="C106:D106"/>
     <mergeCell ref="C108:D108"/>
     <mergeCell ref="C117:D117"/>
-    <mergeCell ref="A113:B113"/>
     <mergeCell ref="C135:D135"/>
     <mergeCell ref="C134:D134"/>
     <mergeCell ref="C136:D136"/>
     <mergeCell ref="C122:D122"/>
     <mergeCell ref="C107:D107"/>
+    <mergeCell ref="A116:E116"/>
+    <mergeCell ref="A117:B117"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="121" priority="6" operator="lessThan">
@@ -15717,10 +15723,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1EAFDB-34A9-4E8B-8792-A6B6BA3CC3A2}">
-  <dimension ref="A1:Y1029"/>
+  <dimension ref="A1:Y1030"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112:D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -15765,8 +15771,8 @@
         <v>138</v>
       </c>
       <c r="C3" s="4">
-        <f>E116</f>
-        <v>3322.71</v>
+        <f>E117</f>
+        <v>3372.71</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -15798,7 +15804,7 @@
       </c>
       <c r="C4" s="55">
         <f>SUM(C3:C3)</f>
-        <v>3322.71</v>
+        <v>3372.71</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -15829,7 +15835,7 @@
         <v>110</v>
       </c>
       <c r="C5" s="55">
-        <f>C86</f>
+        <f>C87</f>
         <v>-8203</v>
       </c>
       <c r="D5" s="5"/>
@@ -15948,7 +15954,7 @@
       <c r="B11" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="255" t="s">
+      <c r="C11" s="254" t="s">
         <v>322</v>
       </c>
       <c r="D11" s="272"/>
@@ -15963,7 +15969,7 @@
       <c r="B12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="255" t="s">
+      <c r="C12" s="254" t="s">
         <v>410</v>
       </c>
       <c r="D12" s="272"/>
@@ -15978,10 +15984,10 @@
       <c r="B13" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C13" s="271" t="s">
+      <c r="C13" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="271"/>
+      <c r="D13" s="270"/>
       <c r="E13" s="65">
         <v>68</v>
       </c>
@@ -15993,10 +15999,10 @@
       <c r="B14" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C14" s="271" t="s">
+      <c r="C14" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="271"/>
+      <c r="D14" s="270"/>
       <c r="E14" s="65">
         <v>68</v>
       </c>
@@ -16016,244 +16022,252 @@
         <v>2405</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="47">
-        <f>SUM(E10:E15)</f>
-        <v>2793</v>
+    <row r="16" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A16" s="32" t="s">
+        <v>412</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>413</v>
+      </c>
+      <c r="C16" s="225" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="226"/>
+      <c r="E16" s="65">
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="13.5" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="47">
+        <f>SUM(E10:E16)</f>
+        <v>2843</v>
+      </c>
     </row>
     <row r="18" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A18" s="230" t="s">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19" spans="1:25" ht="13.5" customHeight="1">
+      <c r="A19" s="230" t="s">
         <v>276</v>
       </c>
-      <c r="B18" s="196"/>
-      <c r="C18" s="196"/>
-      <c r="D18" s="196"/>
-      <c r="E18" s="197"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-    </row>
-    <row r="19" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A19" s="14" t="s">
+      <c r="B19" s="196"/>
+      <c r="C19" s="196"/>
+      <c r="D19" s="196"/>
+      <c r="E19" s="197"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+    </row>
+    <row r="20" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A20" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B20" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="231" t="s">
+      <c r="C20" s="231" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="166"/>
-      <c r="E19" s="16" t="s">
+      <c r="D20" s="166"/>
+      <c r="E20" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A20" s="29" t="s">
+    <row r="21" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A21" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B21" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="270" t="s">
+      <c r="C21" s="271" t="s">
         <v>113</v>
       </c>
-      <c r="D20" s="219"/>
-      <c r="E20" s="26">
+      <c r="D21" s="219"/>
+      <c r="E21" s="26">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="17.25" customHeight="1">
-      <c r="A21" s="32" t="s">
+    <row r="22" spans="1:25" ht="17.25" customHeight="1">
+      <c r="A22" s="32" t="s">
         <v>380</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B22" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C21" s="271" t="s">
+      <c r="C22" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="271"/>
-      <c r="E21" s="65">
+      <c r="D22" s="270"/>
+      <c r="E22" s="65">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A22" s="32" t="s">
+    <row r="23" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A23" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B23" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="225" t="s">
+      <c r="C23" s="225" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="226"/>
-      <c r="E22" s="65">
+      <c r="D23" s="226"/>
+      <c r="E23" s="65">
         <v>2405</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="12">
-        <f>SUM(E20:E22)</f>
-        <v>2473</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="13.5" customHeight="1">
+    <row r="24" spans="1:25" ht="13.15" customHeight="1">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="50"/>
+      <c r="D24" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="12">
+        <f>SUM(E21:E23)</f>
+        <v>2473</v>
+      </c>
     </row>
     <row r="25" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A25" s="230" t="s">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="50"/>
+    </row>
+    <row r="26" spans="1:25" ht="13.5" customHeight="1">
+      <c r="A26" s="230" t="s">
         <v>279</v>
       </c>
-      <c r="B25" s="196"/>
-      <c r="C25" s="196"/>
-      <c r="D25" s="196"/>
-      <c r="E25" s="197"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13"/>
-      <c r="W25" s="13"/>
-      <c r="X25" s="13"/>
-      <c r="Y25" s="13"/>
-    </row>
-    <row r="26" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A26" s="68" t="s">
+      <c r="B26" s="196"/>
+      <c r="C26" s="196"/>
+      <c r="D26" s="196"/>
+      <c r="E26" s="197"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="13"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
+      <c r="Y26" s="13"/>
+    </row>
+    <row r="27" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A27" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="69" t="s">
+      <c r="B27" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="250" t="s">
+      <c r="C27" s="249" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="219"/>
-      <c r="E26" s="70" t="s">
+      <c r="D27" s="219"/>
+      <c r="E27" s="70" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A27" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="154" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="251"/>
-      <c r="E27" s="65">
-        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="13.15" customHeight="1">
       <c r="A28" s="32" t="s">
-        <v>382</v>
+        <v>119</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>379</v>
-      </c>
-      <c r="C28" s="225" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="226"/>
+        <v>25</v>
+      </c>
+      <c r="C28" s="154" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="250"/>
       <c r="E28" s="65">
-        <v>68</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="13.15" customHeight="1">
       <c r="A29" s="32" t="s">
-        <v>143</v>
+        <v>382</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>5</v>
+        <v>379</v>
       </c>
       <c r="C29" s="225" t="s">
         <v>6</v>
       </c>
       <c r="D29" s="226"/>
       <c r="E29" s="65">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A30" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="225" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="226"/>
+      <c r="E30" s="65">
         <v>2405</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="13.15" customHeight="1">
-      <c r="A30" s="44"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="46" t="s">
+    <row r="31" spans="1:25" ht="13.15" customHeight="1">
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="47">
-        <f>SUM(E27:E29)</f>
+      <c r="E31" s="47">
+        <f>SUM(E28:E30)</f>
         <v>2473</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="50"/>
-    </row>
-    <row r="32" spans="1:25" ht="13.15" customHeight="1">
+    <row r="32" spans="1:25" ht="13.5" customHeight="1">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="1"/>
       <c r="D32" s="49"/>
       <c r="E32" s="50"/>
     </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1">
+    <row r="33" spans="1:5" ht="13.15" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="1"/>
@@ -16263,105 +16277,103 @@
     <row r="34" spans="1:5" ht="13.5" customHeight="1">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
     </row>
     <row r="35" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A35" s="249" t="s">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A36" s="248" t="s">
         <v>89</v>
       </c>
-      <c r="B35" s="165"/>
-      <c r="C35" s="166"/>
-    </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A36" s="19" t="s">
+      <c r="B36" s="165"/>
+      <c r="C36" s="166"/>
+    </row>
+    <row r="37" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A37" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B37" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C37" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="21"/>
-    </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A37" s="167" t="s">
+      <c r="D37" s="21"/>
+    </row>
+    <row r="38" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A38" s="167" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="165"/>
-      <c r="C37" s="166"/>
-    </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A38" s="24" t="s">
+      <c r="B38" s="165"/>
+      <c r="C38" s="166"/>
+    </row>
+    <row r="39" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A39" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="18">
+      <c r="B39" s="2"/>
+      <c r="C39" s="18">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A39" s="29" t="s">
+    <row r="40" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A40" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="26">
+      <c r="B40" s="25"/>
+      <c r="C40" s="26">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A40" s="25" t="s">
+    <row r="41" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A41" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B41" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="26">
+      <c r="C41" s="26">
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A41" s="27"/>
-      <c r="B41" s="24" t="s">
+    <row r="42" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A42" s="27"/>
+      <c r="B42" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="28">
-        <f>SUM(C38:C40)</f>
+      <c r="C42" s="28">
+        <f>SUM(C39:C41)</f>
         <v>227</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A42" s="211" t="s">
+    <row r="43" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A43" s="211" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="212"/>
-      <c r="C42" s="213"/>
-    </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A43" s="214"/>
-      <c r="B43" s="215"/>
-      <c r="C43" s="216"/>
+      <c r="B43" s="212"/>
+      <c r="C43" s="213"/>
     </row>
     <row r="44" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A44" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="17">
-        <v>0</v>
-      </c>
+      <c r="A44" s="214"/>
+      <c r="B44" s="215"/>
+      <c r="C44" s="216"/>
     </row>
     <row r="45" spans="1:5" ht="13.5" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="9">
+      <c r="C45" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="13.5" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="9">
@@ -16370,7 +16382,7 @@
     </row>
     <row r="47" spans="1:5" ht="13.5" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="9">
@@ -16379,7 +16391,7 @@
     </row>
     <row r="48" spans="1:5" ht="13.5" customHeight="1">
       <c r="A48" s="2" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="9">
@@ -16387,85 +16399,85 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2" t="s">
+      <c r="A49" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C49" s="9">
-        <f>SUM(C44:C48)</f>
+      <c r="C50" s="9">
+        <f>SUM(C45:C49)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A50" s="167" t="s">
+    <row r="51" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A51" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="165"/>
-      <c r="C50" s="166"/>
-    </row>
-    <row r="51" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A51" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="18">
-        <v>0</v>
-      </c>
+      <c r="B51" s="165"/>
+      <c r="C51" s="166"/>
     </row>
     <row r="52" spans="1:3" ht="13.5" customHeight="1">
       <c r="A52" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C52" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A53" s="2"/>
-      <c r="B53" s="24" t="s">
+      <c r="A53" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A54" s="2"/>
+      <c r="B54" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C53" s="18">
-        <f>SUM(C51:C52)</f>
+      <c r="C54" s="18">
+        <f>SUM(C52:C53)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A54" s="167" t="s">
+    <row r="55" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A55" s="167" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="185"/>
-      <c r="C54" s="186"/>
-    </row>
-    <row r="55" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A55" s="2" t="s">
+      <c r="B55" s="185"/>
+      <c r="C55" s="186"/>
+    </row>
+    <row r="56" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A56" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A56" s="25"/>
-      <c r="B56" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="C56" s="30">
+      <c r="C56" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.5" customHeight="1">
       <c r="A57" s="25"/>
-      <c r="B57" s="25" t="s">
-        <v>79</v>
+      <c r="B57" s="29" t="s">
+        <v>66</v>
       </c>
       <c r="C57" s="30">
         <v>0</v>
@@ -16473,635 +16485,640 @@
     </row>
     <row r="58" spans="1:3" ht="13.5" customHeight="1">
       <c r="A58" s="25"/>
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A59" s="25"/>
+      <c r="B59" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C58" s="30">
-        <f>SUM(C55:C57)</f>
+      <c r="C59" s="30">
+        <f>SUM(C56:C58)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A59" s="167" t="s">
+    <row r="60" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A60" s="167" t="s">
         <v>22</v>
       </c>
-      <c r="B59" s="185"/>
-      <c r="C59" s="186"/>
-    </row>
-    <row r="60" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A60" s="2" t="s">
+      <c r="B60" s="185"/>
+      <c r="C60" s="186"/>
+    </row>
+    <row r="61" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A61" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B61" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C60" s="17">
+      <c r="C61" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A61" s="25"/>
-      <c r="B61" s="29" t="s">
+    <row r="62" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A62" s="25"/>
+      <c r="B62" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C61" s="30">
-        <f>SUM(C60)</f>
+      <c r="C62" s="30">
+        <f>SUM(C61)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A62" s="217" t="s">
+    <row r="63" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A63" s="217" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="218"/>
-      <c r="C62" s="219"/>
-    </row>
-    <row r="63" spans="1:3" ht="33" customHeight="1">
-      <c r="A63" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="B63" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="C63" s="33">
-        <v>0</v>
-      </c>
+      <c r="B63" s="218"/>
+      <c r="C63" s="219"/>
     </row>
     <row r="64" spans="1:3" ht="33" customHeight="1">
       <c r="A64" s="31" t="s">
-        <v>259</v>
+        <v>55</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>260</v>
+        <v>56</v>
       </c>
       <c r="C64" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="30">
+    <row r="65" spans="1:3" ht="33" customHeight="1">
       <c r="A65" s="31" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C65" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="33" customHeight="1">
+    <row r="66" spans="1:3" ht="30">
       <c r="A66" s="31" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C66" s="33">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="19.899999999999999" customHeight="1">
-      <c r="A67" s="31"/>
+    <row r="67" spans="1:3" ht="33" customHeight="1">
+      <c r="A67" s="31" t="s">
+        <v>261</v>
+      </c>
       <c r="B67" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="C67" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A68" s="31"/>
+      <c r="B68" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C67" s="33">
-        <f>SUM(C63:C66)</f>
+      <c r="C68" s="33">
+        <f>SUM(C64:C67)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A68" s="223" t="s">
+    <row r="69" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A69" s="223" t="s">
         <v>35</v>
       </c>
-      <c r="B68" s="215"/>
-      <c r="C68" s="197"/>
-    </row>
-    <row r="69" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A69" s="25" t="s">
+      <c r="B69" s="215"/>
+      <c r="C69" s="197"/>
+    </row>
+    <row r="70" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A70" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B69" s="25"/>
-      <c r="C69" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="15" customHeight="1">
-      <c r="A70" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="B70" s="27" t="s">
-        <v>64</v>
-      </c>
+      <c r="B70" s="25"/>
       <c r="C70" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A71" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>26</v>
+    <row r="71" spans="1:3" ht="15" customHeight="1">
+      <c r="A71" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B71" s="27" t="s">
+        <v>64</v>
       </c>
       <c r="C71" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A72" s="31"/>
-      <c r="B72" s="32" t="s">
+      <c r="A72" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A73" s="31"/>
+      <c r="B73" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C72" s="33">
-        <f>SUM(C69:C71)</f>
+      <c r="C73" s="33">
+        <f>SUM(C70:C72)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A73" s="198" t="s">
+    <row r="74" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A74" s="198" t="s">
         <v>31</v>
       </c>
-      <c r="B73" s="222"/>
-      <c r="C73" s="200"/>
-    </row>
-    <row r="74" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A74" s="56" t="s">
+      <c r="B74" s="222"/>
+      <c r="C74" s="200"/>
+    </row>
+    <row r="75" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A75" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B74" s="61" t="s">
+      <c r="B75" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="C74" s="58">
+      <c r="C75" s="58">
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A75" s="66" t="s">
+    <row r="76" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A76" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="76" t="s">
+      <c r="B76" s="76" t="s">
         <v>111</v>
       </c>
-      <c r="C75" s="67">
+      <c r="C76" s="67">
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="57" t="s">
+    <row r="77" spans="1:3">
+      <c r="A77" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="B76" s="114" t="s">
+      <c r="B77" s="114" t="s">
         <v>310</v>
       </c>
-      <c r="C76" s="59">
+      <c r="C77" s="59">
         <v>52</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A77" s="29" t="s">
+    <row r="78" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A78" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B77" s="60" t="s">
+      <c r="B78" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="C77" s="30">
+      <c r="C78" s="30">
         <v>900</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A78" s="27"/>
-      <c r="B78" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C78" s="38">
-        <f>SUM(C74:C77)</f>
-        <v>1160</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="13.5" customHeight="1">
       <c r="A79" s="27"/>
-      <c r="B79" s="52" t="s">
+      <c r="B79" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C79" s="38">
+        <f>SUM(C75:C78)</f>
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A80" s="27"/>
+      <c r="B80" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="C79" s="38">
-        <f>C41+C49+C53+C58+C61+C67+C72+C78</f>
+      <c r="C80" s="38">
+        <f>C42+C50+C54+C59+C62+C68+C73+C79</f>
         <v>1387</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A80" s="198" t="s">
+    <row r="81" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A81" s="198" t="s">
         <v>44</v>
       </c>
-      <c r="B80" s="199"/>
-      <c r="C80" s="200"/>
-    </row>
-    <row r="81" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A81" s="41" t="s">
+      <c r="B81" s="199"/>
+      <c r="C81" s="200"/>
+    </row>
+    <row r="82" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A82" s="41" t="s">
         <v>47</v>
-      </c>
-      <c r="B81" s="37"/>
-      <c r="C81" s="123">
-        <f>IF(('July 2024 - September 2024'!C91)+SUM(E95+E103+E113)  &lt; 0,(('July 2024 - September 2024'!C91))+SUM(E95+E103+E113), TEXT((('July 2024 - September 2024'!C91))+SUM(E95+E103+E113),"+$0.00"))</f>
-        <v>-7903</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A82" s="103" t="s">
-        <v>255</v>
       </c>
       <c r="B82" s="37"/>
       <c r="C82" s="123">
-        <v>0</v>
+        <f>IF(('July 2024 - September 2024'!C91)+SUM(E96+E104+E114)  &lt; 0,(('July 2024 - September 2024'!C91))+SUM(E96+E104+E114), TEXT((('July 2024 - September 2024'!C91))+SUM(E96+E104+E114),"+$0.00"))</f>
+        <v>-7903</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A83" s="101" t="s">
-        <v>247</v>
+      <c r="A83" s="103" t="s">
+        <v>255</v>
       </c>
       <c r="B83" s="37"/>
       <c r="C83" s="123">
-        <f>IF(('July 2024 - September 2024'!C93)+SUM(E94+E104) &lt; 0,(('July 2024 - September 2024'!C93))+SUM(E94+E104), TEXT((('July 2024 - September 2024'!C93))+SUM(E94+E104),"+$0.00"))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A84" s="101" t="s">
+        <v>247</v>
+      </c>
+      <c r="B84" s="37"/>
+      <c r="C84" s="123">
+        <f>IF(('July 2024 - September 2024'!C93)+SUM(E95+E105) &lt; 0,(('July 2024 - September 2024'!C93))+SUM(E95+E105), TEXT((('July 2024 - September 2024'!C93))+SUM(E95+E105),"+$0.00"))</f>
         <v>-300</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="30">
-      <c r="A84" s="63" t="s">
+    <row r="85" spans="1:8" ht="30">
+      <c r="A85" s="63" t="s">
         <v>70</v>
-      </c>
-      <c r="B84" s="53"/>
-      <c r="C84" s="123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="30">
-      <c r="A85" s="77" t="s">
-        <v>112</v>
       </c>
       <c r="B85" s="53"/>
       <c r="C85" s="123">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A86" s="27"/>
-      <c r="B86" s="54" t="s">
+    <row r="86" spans="1:8" ht="30">
+      <c r="A86" s="77" t="s">
+        <v>112</v>
+      </c>
+      <c r="B86" s="53"/>
+      <c r="C86" s="123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A87" s="27"/>
+      <c r="B87" s="54" t="s">
         <v>319</v>
       </c>
-      <c r="C86" s="48">
-        <f>C81+C82+C83+C84+C85</f>
+      <c r="C87" s="48">
+        <f>C82+C83+C84+C85+C86</f>
         <v>-8203</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A87" s="31"/>
-      <c r="B87" s="39" t="s">
+    <row r="88" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A88" s="31"/>
+      <c r="B88" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C87" s="40">
-        <f>C79</f>
+      <c r="C88" s="40">
+        <f>C80</f>
         <v>1387</v>
       </c>
-      <c r="H87" s="35"/>
-    </row>
-    <row r="88" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A88" s="10"/>
-      <c r="B88" s="10"/>
+      <c r="H88" s="35"/>
     </row>
     <row r="89" spans="1:8" ht="13.5" customHeight="1">
       <c r="A89" s="10"/>
       <c r="B89" s="10"/>
     </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="168" t="s">
+    <row r="90" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A90" s="10"/>
+      <c r="B90" s="10"/>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" s="168" t="s">
         <v>300</v>
       </c>
-      <c r="B90" s="165"/>
-      <c r="C90" s="165"/>
-      <c r="D90" s="165"/>
-      <c r="E90" s="166"/>
-      <c r="G90" s="115" t="s">
+      <c r="B91" s="165"/>
+      <c r="C91" s="165"/>
+      <c r="D91" s="165"/>
+      <c r="E91" s="166"/>
+      <c r="G91" s="115" t="s">
         <v>316</v>
       </c>
-      <c r="H90" s="118">
+      <c r="H91" s="118">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="60">
-      <c r="A91" s="174" t="s">
+    <row r="92" spans="1:8" ht="60">
+      <c r="A92" s="174" t="s">
         <v>38</v>
       </c>
-      <c r="B91" s="219"/>
-      <c r="C91" s="174" t="s">
+      <c r="B92" s="219"/>
+      <c r="C92" s="174" t="s">
         <v>37</v>
       </c>
-      <c r="D91" s="219"/>
-      <c r="E91" s="42" t="s">
+      <c r="D92" s="219"/>
+      <c r="E92" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="G91" s="116" t="s">
+      <c r="G92" s="116" t="s">
         <v>317</v>
       </c>
-      <c r="H91" s="117">
-        <f>C74-H90</f>
+      <c r="H92" s="117">
+        <f>C75-H91</f>
         <v>140</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A92" s="193" t="s">
+    <row r="93" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A93" s="193" t="s">
         <v>196</v>
       </c>
-      <c r="B92" s="194"/>
-      <c r="C92" s="269"/>
-      <c r="D92" s="219"/>
-      <c r="E92" s="86">
+      <c r="B93" s="194"/>
+      <c r="C93" s="265"/>
+      <c r="D93" s="219"/>
+      <c r="E93" s="86">
         <f>'July 2024 - September 2024'!E142</f>
         <v>302.71000000000004</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="34.5" customHeight="1">
-      <c r="A93" s="156" t="s">
+    <row r="94" spans="1:8" ht="34.5" customHeight="1">
+      <c r="A94" s="156" t="s">
         <v>73</v>
       </c>
-      <c r="B93" s="157"/>
-      <c r="C93" s="262" t="s">
+      <c r="B94" s="157"/>
+      <c r="C94" s="261" t="s">
         <v>377</v>
       </c>
-      <c r="D93" s="252"/>
-      <c r="E93" s="51">
+      <c r="D94" s="251"/>
+      <c r="E94" s="51">
         <v>150</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A94" s="158"/>
-      <c r="B94" s="159"/>
-      <c r="C94" s="169" t="s">
-        <v>374</v>
-      </c>
-      <c r="D94" s="169"/>
-      <c r="E94" s="51">
-        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="13.5" customHeight="1">
       <c r="A95" s="158"/>
       <c r="B95" s="159"/>
       <c r="C95" s="169" t="s">
-        <v>269</v>
+        <v>374</v>
       </c>
       <c r="D95" s="169"/>
       <c r="E95" s="51">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A96" s="158"/>
+      <c r="B96" s="159"/>
+      <c r="C96" s="169" t="s">
+        <v>269</v>
+      </c>
+      <c r="D96" s="169"/>
+      <c r="E96" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A96" s="160"/>
-      <c r="B96" s="161"/>
-      <c r="C96" s="162" t="s">
+    <row r="97" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A97" s="160"/>
+      <c r="B97" s="161"/>
+      <c r="C97" s="162" t="s">
         <v>411</v>
       </c>
-      <c r="D96" s="163"/>
-      <c r="E96" s="51">
+      <c r="D97" s="163"/>
+      <c r="E97" s="51">
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A97" s="160" t="s">
+    <row r="98" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A98" s="160" t="s">
         <v>40</v>
       </c>
-      <c r="B97" s="161"/>
-      <c r="C97" s="245"/>
-      <c r="D97" s="245"/>
-      <c r="E97" s="74">
-        <f>C87</f>
+      <c r="B98" s="161"/>
+      <c r="C98" s="244"/>
+      <c r="D98" s="244"/>
+      <c r="E98" s="74">
+        <f>C88</f>
         <v>1387</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="13.5" customHeight="1">
-      <c r="C98" s="248" t="s">
+    <row r="99" spans="1:8" ht="13.5" customHeight="1">
+      <c r="C99" s="247" t="s">
         <v>41</v>
       </c>
-      <c r="D98" s="215"/>
-      <c r="E98" s="73">
-        <f>('July 2024 - September 2024'!E142+E16)-SUM(E93:E97)</f>
-        <v>1300.71</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="13.5" customHeight="1"/>
-    <row r="100" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A100" s="168" t="s">
+      <c r="D99" s="215"/>
+      <c r="E99" s="73">
+        <f>('July 2024 - September 2024'!E142+E17)-SUM(E94:E98)</f>
+        <v>1350.71</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="13.5" customHeight="1"/>
+    <row r="101" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A101" s="168" t="s">
         <v>150</v>
       </c>
-      <c r="B100" s="165"/>
-      <c r="C100" s="165"/>
-      <c r="D100" s="165"/>
-      <c r="E100" s="166"/>
-      <c r="G100" s="115" t="s">
+      <c r="B101" s="165"/>
+      <c r="C101" s="165"/>
+      <c r="D101" s="165"/>
+      <c r="E101" s="166"/>
+      <c r="G101" s="115" t="s">
         <v>316</v>
       </c>
-      <c r="H100" s="118">
+      <c r="H101" s="118">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="60">
-      <c r="A101" s="168" t="s">
+    <row r="102" spans="1:8" ht="60">
+      <c r="A102" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="B101" s="166"/>
-      <c r="C101" s="168" t="s">
+      <c r="B102" s="166"/>
+      <c r="C102" s="168" t="s">
         <v>37</v>
       </c>
-      <c r="D101" s="166"/>
-      <c r="E101" s="22" t="s">
+      <c r="D102" s="166"/>
+      <c r="E102" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G101" s="116" t="s">
+      <c r="G102" s="116" t="s">
         <v>317</v>
       </c>
-      <c r="H101" s="117">
-        <f>C74-H100</f>
+      <c r="H102" s="117">
+        <f>C75-H101</f>
         <v>140</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A102" s="205" t="s">
+    <row r="103" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A103" s="205" t="s">
         <v>87</v>
       </c>
-      <c r="B102" s="229"/>
-      <c r="C102" s="263"/>
-      <c r="D102" s="264"/>
-      <c r="E102" s="36">
-        <f>E98</f>
-        <v>1300.71</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A103" s="193" t="s">
+      <c r="B103" s="229"/>
+      <c r="C103" s="262"/>
+      <c r="D103" s="263"/>
+      <c r="E103" s="36">
+        <f>E99</f>
+        <v>1350.71</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A104" s="193" t="s">
         <v>73</v>
       </c>
-      <c r="B103" s="265"/>
-      <c r="C103" s="187" t="s">
+      <c r="B104" s="266"/>
+      <c r="C104" s="187" t="s">
         <v>74</v>
       </c>
-      <c r="D103" s="261"/>
-      <c r="E103" s="51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A104" s="266"/>
-      <c r="B104" s="267"/>
-      <c r="C104" s="189" t="s">
-        <v>326</v>
-      </c>
-      <c r="D104" s="173"/>
+      <c r="D104" s="269"/>
       <c r="E104" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="12.75" customHeight="1">
-      <c r="A105" s="201"/>
+    <row r="105" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A105" s="267"/>
       <c r="B105" s="268"/>
-      <c r="C105" s="262" t="s">
+      <c r="C105" s="189" t="s">
+        <v>326</v>
+      </c>
+      <c r="D105" s="173"/>
+      <c r="E105" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A106" s="201"/>
+      <c r="B106" s="264"/>
+      <c r="C106" s="261" t="s">
         <v>325</v>
       </c>
-      <c r="D105" s="169"/>
-      <c r="E105" s="71">
+      <c r="D106" s="162"/>
+      <c r="E106" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A106" s="205" t="s">
+    <row r="107" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A107" s="205" t="s">
         <v>40</v>
       </c>
-      <c r="B106" s="229"/>
-      <c r="C106" s="257"/>
-      <c r="D106" s="197"/>
-      <c r="E106" s="64">
-        <f>C87</f>
+      <c r="B107" s="229"/>
+      <c r="C107" s="256"/>
+      <c r="D107" s="215"/>
+      <c r="E107" s="74">
+        <f>C88</f>
         <v>1387</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="13.5" customHeight="1">
-      <c r="C107" s="192" t="s">
+    <row r="108" spans="1:8" ht="13.5" customHeight="1">
+      <c r="C108" s="192" t="s">
         <v>28</v>
       </c>
-      <c r="D107" s="166"/>
-      <c r="E107" s="36">
-        <f>(E23+E102)-SUM(E103:E106)</f>
-        <v>2386.71</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A108" s="23"/>
-      <c r="B108" s="23"/>
-      <c r="C108" s="23"/>
-      <c r="D108" s="23"/>
-      <c r="E108" s="23"/>
-    </row>
-    <row r="109" spans="1:8" ht="17.25" customHeight="1">
+      <c r="D108" s="166"/>
+      <c r="E108" s="36">
+        <f>(E24+E103)-SUM(E104:E107)</f>
+        <v>2436.71</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="13.5" customHeight="1">
       <c r="A109" s="23"/>
       <c r="B109" s="23"/>
       <c r="C109" s="23"/>
       <c r="D109" s="23"/>
       <c r="E109" s="23"/>
     </row>
-    <row r="110" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A110" s="195" t="s">
+    <row r="110" spans="1:8" ht="17.25" customHeight="1">
+      <c r="A110" s="23"/>
+      <c r="B110" s="23"/>
+      <c r="C110" s="23"/>
+      <c r="D110" s="23"/>
+      <c r="E110" s="23"/>
+    </row>
+    <row r="111" spans="1:8" ht="13.5" customHeight="1">
+      <c r="A111" s="195" t="s">
         <v>151</v>
       </c>
-      <c r="B110" s="196"/>
-      <c r="C110" s="196"/>
-      <c r="D110" s="196"/>
-      <c r="E110" s="197"/>
-      <c r="G110" s="115" t="s">
+      <c r="B111" s="196"/>
+      <c r="C111" s="196"/>
+      <c r="D111" s="196"/>
+      <c r="E111" s="197"/>
+      <c r="G111" s="115" t="s">
         <v>316</v>
       </c>
-      <c r="H110" s="118">
+      <c r="H111" s="118">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="60">
-      <c r="A111" s="168" t="s">
+    <row r="112" spans="1:8" ht="60">
+      <c r="A112" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="B111" s="166"/>
-      <c r="C111" s="168" t="s">
+      <c r="B112" s="166"/>
+      <c r="C112" s="168" t="s">
         <v>37</v>
       </c>
-      <c r="D111" s="166"/>
-      <c r="E111" s="22" t="s">
+      <c r="D112" s="166"/>
+      <c r="E112" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G111" s="116" t="s">
+      <c r="G112" s="116" t="s">
         <v>317</v>
       </c>
-      <c r="H111" s="117">
-        <f>C74-H110</f>
+      <c r="H112" s="117">
+        <f>C75-H111</f>
         <v>140</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A112" s="205" t="s">
+    <row r="113" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A113" s="205" t="s">
         <v>90</v>
       </c>
-      <c r="B112" s="229"/>
-      <c r="C112" s="182"/>
-      <c r="D112" s="166"/>
-      <c r="E112" s="36">
-        <f>E107</f>
-        <v>2386.71</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A113" s="193" t="s">
+      <c r="B113" s="229"/>
+      <c r="C113" s="182"/>
+      <c r="D113" s="166"/>
+      <c r="E113" s="36">
+        <f>E108</f>
+        <v>2436.71</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A114" s="193" t="s">
         <v>73</v>
       </c>
-      <c r="B113" s="176"/>
-      <c r="C113" s="189" t="s">
+      <c r="B114" s="176"/>
+      <c r="C114" s="189" t="s">
         <v>74</v>
       </c>
-      <c r="D113" s="256"/>
-      <c r="E113" s="51">
+      <c r="D114" s="255"/>
+      <c r="E114" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="38.25" customHeight="1">
-      <c r="A114" s="201"/>
-      <c r="B114" s="268"/>
-      <c r="C114" s="262" t="s">
+    <row r="115" spans="1:5" ht="38.25" customHeight="1">
+      <c r="A115" s="201"/>
+      <c r="B115" s="264"/>
+      <c r="C115" s="261" t="s">
         <v>383</v>
       </c>
-      <c r="D114" s="169"/>
-      <c r="E114" s="71">
+      <c r="D115" s="162"/>
+      <c r="E115" s="51">
         <v>150</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A115" s="205" t="s">
+    <row r="116" spans="1:5" ht="13.5" customHeight="1">
+      <c r="A116" s="205" t="s">
         <v>40</v>
       </c>
-      <c r="B115" s="229"/>
-      <c r="C115" s="257"/>
-      <c r="D115" s="197"/>
-      <c r="E115" s="64">
-        <f>C87</f>
+      <c r="B116" s="229"/>
+      <c r="C116" s="256"/>
+      <c r="D116" s="215"/>
+      <c r="E116" s="74">
+        <f>C88</f>
         <v>1387</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="13.5" customHeight="1">
-      <c r="C116" s="192" t="s">
+    <row r="117" spans="1:5" ht="13.5" customHeight="1">
+      <c r="C117" s="192" t="s">
         <v>28</v>
       </c>
-      <c r="D116" s="166"/>
-      <c r="E116" s="51">
-        <f>(E30+E112)-SUM(E113:E115)</f>
-        <v>3322.71</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" ht="13.5" customHeight="1">
-      <c r="A117" s="10"/>
-      <c r="B117" s="10"/>
+      <c r="D117" s="166"/>
+      <c r="E117" s="51">
+        <f>(E31+E113)-SUM(E114:E116)</f>
+        <v>3372.71</v>
+      </c>
     </row>
     <row r="118" spans="1:5" ht="13.5" customHeight="1">
       <c r="A118" s="10"/>
@@ -20751,73 +20768,78 @@
       <c r="A1029" s="10"/>
       <c r="B1029" s="10"/>
     </row>
+    <row r="1030" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A1030" s="10"/>
+      <c r="B1030" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="65">
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
+  <mergeCells count="66">
+    <mergeCell ref="C16:D16"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A80:C80"/>
-    <mergeCell ref="A90:E90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="A81:C81"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A91:E91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="C92:D92"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C29:D29"/>
-    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A69:C69"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A43:C44"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A94:B97"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="A104:B106"/>
     <mergeCell ref="C104:D104"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="A93:B96"/>
+    <mergeCell ref="C106:D106"/>
     <mergeCell ref="C96:D96"/>
-    <mergeCell ref="A103:B105"/>
-    <mergeCell ref="A113:B114"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="A116:B116"/>
     <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="A100:E100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="A103:B103"/>
     <mergeCell ref="C112:D112"/>
+    <mergeCell ref="A107:B107"/>
     <mergeCell ref="C107:D107"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A111:E111"/>
     <mergeCell ref="C115:D115"/>
     <mergeCell ref="C103:D103"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="A42:C43"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A110:E110"/>
+    <mergeCell ref="A114:B115"/>
+    <mergeCell ref="C117:D117"/>
     <mergeCell ref="C94:D94"/>
     <mergeCell ref="C114:D114"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="A102:B102"/>
     <mergeCell ref="C102:D102"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="A112:B112"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="106" priority="9" operator="lessThan">
@@ -20832,7 +20854,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C81:C85">
+  <conditionalFormatting sqref="C82:C86">
     <cfRule type="cellIs" dxfId="103" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -20840,7 +20862,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
+  <conditionalFormatting sqref="E93">
     <cfRule type="cellIs" dxfId="101" priority="6" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20848,7 +20870,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E98">
+  <conditionalFormatting sqref="E99">
     <cfRule type="cellIs" dxfId="99" priority="18" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20856,7 +20878,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E102">
+  <conditionalFormatting sqref="E103">
     <cfRule type="cellIs" dxfId="97" priority="14" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20864,7 +20886,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E107">
+  <conditionalFormatting sqref="E108">
     <cfRule type="cellIs" dxfId="95" priority="16" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20872,7 +20894,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E112">
+  <conditionalFormatting sqref="E113">
     <cfRule type="cellIs" dxfId="93" priority="12" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20880,7 +20902,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E116">
+  <conditionalFormatting sqref="E117">
     <cfRule type="cellIs" dxfId="91" priority="10" stopIfTrue="1" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
@@ -20896,8 +20918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5AAEA1-C3EE-4B36-938E-0F583AF15471}">
   <dimension ref="A1:Y1023"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90:D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -20943,7 +20965,7 @@
       </c>
       <c r="C3" s="4">
         <f>E110</f>
-        <v>841.86999999999989</v>
+        <v>891.86999999999989</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -20975,7 +20997,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>841.86999999999989</v>
+        <v>891.86999999999989</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -21125,10 +21147,10 @@
       <c r="B11" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C11" s="271" t="s">
+      <c r="C11" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="271"/>
+      <c r="D11" s="270"/>
       <c r="E11" s="65">
         <v>68</v>
       </c>
@@ -21229,10 +21251,10 @@
       <c r="B18" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C18" s="271" t="s">
+      <c r="C18" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="271"/>
+      <c r="D18" s="270"/>
       <c r="E18" s="65">
         <v>68</v>
       </c>
@@ -21306,7 +21328,7 @@
       <c r="B23" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="250" t="s">
+      <c r="C23" s="249" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="219"/>
@@ -21339,7 +21361,7 @@
       <c r="C25" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="251"/>
+      <c r="D25" s="250"/>
       <c r="E25" s="65">
         <v>0</v>
       </c>
@@ -21382,7 +21404,7 @@
       <c r="B30" s="10"/>
     </row>
     <row r="31" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A31" s="249" t="s">
+      <c r="A31" s="248" t="s">
         <v>95</v>
       </c>
       <c r="B31" s="165"/>
@@ -21819,7 +21841,7 @@
       </c>
       <c r="B77" s="37"/>
       <c r="C77" s="123">
-        <f>IF(('October 2024 - December 2024'!C81)+SUM(E88+E90+E99+E107)  &lt; 0,(('October 2024 - December 2024'!C81))+SUM(E88+E90+E99+E107), TEXT((('October 2024 - December 2024'!C81))+SUM(E88+E90+E99+E107),"+$0.00"))</f>
+        <f>IF(('October 2024 - December 2024'!C82)+SUM(E88+E90+E99+E107)  &lt; 0,(('October 2024 - December 2024'!C82))+SUM(E88+E90+E99+E107), TEXT((('October 2024 - December 2024'!C82))+SUM(E88+E90+E99+E107),"+$0.00"))</f>
         <v>-5800</v>
       </c>
     </row>
@@ -21838,7 +21860,7 @@
       </c>
       <c r="B79" s="37"/>
       <c r="C79" s="123" t="str">
-        <f>IF(('October 2024 - December 2024'!C83)+SUM(E89) &lt; 0,(('October 2024 - December 2024'!C83))+SUM(E89), TEXT((('October 2024 - December 2024'!C83))+SUM(E89),"+$0.00"))</f>
+        <f>IF(('October 2024 - December 2024'!C84)+SUM(E89) &lt; 0,(('October 2024 - December 2024'!C84))+SUM(E89), TEXT((('October 2024 - December 2024'!C84))+SUM(E89),"+$0.00"))</f>
         <v>+$0.00</v>
       </c>
     </row>
@@ -21932,7 +21954,7 @@
       <c r="C88" s="169" t="s">
         <v>405</v>
       </c>
-      <c r="D88" s="252"/>
+      <c r="D88" s="251"/>
       <c r="E88" s="51">
         <v>100</v>
       </c>
@@ -21951,10 +21973,10 @@
     <row r="90" spans="1:8" ht="19.5" customHeight="1">
       <c r="A90" s="158"/>
       <c r="B90" s="159"/>
-      <c r="C90" s="262" t="s">
+      <c r="C90" s="261" t="s">
         <v>375</v>
       </c>
-      <c r="D90" s="262"/>
+      <c r="D90" s="261"/>
       <c r="E90" s="51">
         <v>1003</v>
       </c>
@@ -21965,7 +21987,7 @@
       <c r="C91" s="281" t="s">
         <v>376</v>
       </c>
-      <c r="D91" s="258"/>
+      <c r="D91" s="257"/>
       <c r="E91" s="51">
         <v>0</v>
       </c>
@@ -21975,21 +21997,21 @@
         <v>40</v>
       </c>
       <c r="B92" s="161"/>
-      <c r="C92" s="245"/>
-      <c r="D92" s="245"/>
+      <c r="C92" s="244"/>
+      <c r="D92" s="244"/>
       <c r="E92" s="74">
         <f>C83</f>
         <v>1387</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="13.5" customHeight="1">
-      <c r="C93" s="248" t="s">
+      <c r="C93" s="247" t="s">
         <v>41</v>
       </c>
       <c r="D93" s="215"/>
       <c r="E93" s="36">
-        <f>('October 2024 - December 2024'!E116+E13)-SUM(E88:E92)</f>
-        <v>3005.71</v>
+        <f>('October 2024 - December 2024'!E117+E13)-SUM(E88:E92)</f>
+        <v>3055.71</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1"/>
@@ -22033,18 +22055,18 @@
         <v>100</v>
       </c>
       <c r="B97" s="229"/>
-      <c r="C97" s="263"/>
-      <c r="D97" s="264"/>
+      <c r="C97" s="262"/>
+      <c r="D97" s="263"/>
       <c r="E97" s="36">
         <f>E93</f>
-        <v>3005.71</v>
+        <v>3055.71</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="88.5" customHeight="1">
       <c r="A98" s="193" t="s">
         <v>73</v>
       </c>
-      <c r="B98" s="265"/>
+      <c r="B98" s="266"/>
       <c r="C98" s="277" t="s">
         <v>407</v>
       </c>
@@ -22059,7 +22081,7 @@
       <c r="C99" s="187" t="s">
         <v>335</v>
       </c>
-      <c r="D99" s="261"/>
+      <c r="D99" s="269"/>
       <c r="E99" s="51">
         <v>0</v>
       </c>
@@ -22083,7 +22105,7 @@
       <c r="D101" s="166"/>
       <c r="E101" s="36">
         <f>(E20+E97)-SUM(E98:E100)</f>
-        <v>823.86999999999989</v>
+        <v>873.86999999999989</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="13.5" customHeight="1">
@@ -22144,25 +22166,25 @@
       <c r="D106" s="166"/>
       <c r="E106" s="36">
         <f>E101</f>
-        <v>823.86999999999989</v>
+        <v>873.86999999999989</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">
       <c r="A107" s="193" t="s">
         <v>73</v>
       </c>
-      <c r="B107" s="265"/>
+      <c r="B107" s="266"/>
       <c r="C107" s="189" t="s">
         <v>200</v>
       </c>
-      <c r="D107" s="256"/>
+      <c r="D107" s="255"/>
       <c r="E107" s="71">
         <v>1000</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="13.5" customHeight="1">
       <c r="A108" s="201"/>
-      <c r="B108" s="268"/>
+      <c r="B108" s="264"/>
       <c r="C108" s="162" t="s">
         <v>318</v>
       </c>
@@ -22190,7 +22212,7 @@
       <c r="D110" s="197"/>
       <c r="E110" s="100">
         <f>(E26+E106)-SUM(E107:E109)</f>
-        <v>841.86999999999989</v>
+        <v>891.86999999999989</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="13.5" customHeight="1">
@@ -26022,7 +26044,7 @@
       </c>
       <c r="C3" s="4">
         <f>E109</f>
-        <v>1099.8699999999999</v>
+        <v>1149.8699999999999</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -26054,7 +26076,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>1099.8699999999999</v>
+        <v>1149.8699999999999</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -26204,10 +26226,10 @@
       <c r="B11" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C11" s="271" t="s">
+      <c r="C11" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="271"/>
+      <c r="D11" s="270"/>
       <c r="E11" s="65">
         <v>68</v>
       </c>
@@ -26308,10 +26330,10 @@
       <c r="B18" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C18" s="271" t="s">
+      <c r="C18" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="271"/>
+      <c r="D18" s="270"/>
       <c r="E18" s="65">
         <v>68</v>
       </c>
@@ -26323,10 +26345,10 @@
       <c r="B19" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C19" s="271" t="s">
+      <c r="C19" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="271"/>
+      <c r="D19" s="270"/>
       <c r="E19" s="65">
         <v>68</v>
       </c>
@@ -26400,7 +26422,7 @@
       <c r="B24" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="250" t="s">
+      <c r="C24" s="249" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="219"/>
@@ -26433,7 +26455,7 @@
       <c r="C26" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="251"/>
+      <c r="D26" s="250"/>
       <c r="E26" s="65">
         <v>0</v>
       </c>
@@ -26476,7 +26498,7 @@
       <c r="B31" s="10"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A32" s="249" t="s">
+      <c r="A32" s="248" t="s">
         <v>97</v>
       </c>
       <c r="B32" s="165"/>
@@ -27027,7 +27049,7 @@
       <c r="C89" s="169" t="s">
         <v>200</v>
       </c>
-      <c r="D89" s="252"/>
+      <c r="D89" s="251"/>
       <c r="E89" s="51">
         <v>1000</v>
       </c>
@@ -27044,12 +27066,12 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A91" s="241" t="s">
+      <c r="A91" s="259" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="241"/>
-      <c r="C91" s="245"/>
-      <c r="D91" s="245"/>
+      <c r="B91" s="259"/>
+      <c r="C91" s="244"/>
+      <c r="D91" s="244"/>
       <c r="E91" s="74">
         <f>C84</f>
         <v>1387</v>
@@ -27058,13 +27080,13 @@
     <row r="92" spans="1:8" ht="13.5" customHeight="1">
       <c r="A92" s="72"/>
       <c r="B92" s="72"/>
-      <c r="C92" s="248" t="s">
+      <c r="C92" s="247" t="s">
         <v>41</v>
       </c>
       <c r="D92" s="215"/>
       <c r="E92" s="73">
         <f>('January 2025 - March 2025'!E110+E13)-SUM(E89:E91)</f>
-        <v>927.86999999999989</v>
+        <v>977.86999999999989</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="13.5" customHeight="1"/>
@@ -27108,22 +27130,22 @@
         <v>98</v>
       </c>
       <c r="B96" s="229"/>
-      <c r="C96" s="263"/>
-      <c r="D96" s="264"/>
+      <c r="C96" s="262"/>
+      <c r="D96" s="263"/>
       <c r="E96" s="36">
         <f>E92</f>
-        <v>927.86999999999989</v>
+        <v>977.86999999999989</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="13.5" customHeight="1">
       <c r="A97" s="193" t="s">
         <v>73</v>
       </c>
-      <c r="B97" s="265"/>
+      <c r="B97" s="266"/>
       <c r="C97" s="187" t="s">
         <v>200</v>
       </c>
-      <c r="D97" s="261"/>
+      <c r="D97" s="269"/>
       <c r="E97" s="51">
         <v>1000</v>
       </c>
@@ -27158,7 +27180,7 @@
       <c r="D100" s="166"/>
       <c r="E100" s="36">
         <f>(E21+E96)-SUM(E97:E99)</f>
-        <v>1081.8699999999999</v>
+        <v>1131.8699999999999</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="13.5" customHeight="1">
@@ -27219,14 +27241,14 @@
       <c r="D105" s="166"/>
       <c r="E105" s="36">
         <f>E100</f>
-        <v>1081.8699999999999</v>
+        <v>1131.8699999999999</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="13.5" customHeight="1">
       <c r="A106" s="193" t="s">
         <v>73</v>
       </c>
-      <c r="B106" s="265"/>
+      <c r="B106" s="266"/>
       <c r="C106" s="187" t="s">
         <v>200</v>
       </c>
@@ -27265,7 +27287,7 @@
       <c r="D109" s="166"/>
       <c r="E109" s="51">
         <f>(E27+E105)-SUM(E106:E108)</f>
-        <v>1099.8699999999999</v>
+        <v>1149.8699999999999</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="13.5" customHeight="1">
@@ -30929,6 +30951,12 @@
     <mergeCell ref="A39:C40"/>
     <mergeCell ref="A47:C47"/>
     <mergeCell ref="A51:C51"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="A59:C59"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A32:C32"/>
     <mergeCell ref="C109:D109"/>
     <mergeCell ref="C100:D100"/>
     <mergeCell ref="A103:E103"/>
@@ -30957,27 +30985,21 @@
     <mergeCell ref="A94:E94"/>
     <mergeCell ref="A96:B96"/>
     <mergeCell ref="C96:D96"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C20:D20"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A32:C32"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C20:D20"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
     <cfRule type="cellIs" dxfId="74" priority="11" operator="lessThan">
@@ -31097,7 +31119,7 @@
       </c>
       <c r="C3" s="4">
         <f>E109</f>
-        <v>1407.87</v>
+        <v>1457.87</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -31129,7 +31151,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>1407.87</v>
+        <v>1457.87</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -31279,10 +31301,10 @@
       <c r="B11" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C11" s="271" t="s">
+      <c r="C11" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="271"/>
+      <c r="D11" s="270"/>
       <c r="E11" s="65">
         <v>68</v>
       </c>
@@ -31294,10 +31316,10 @@
       <c r="B12" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C12" s="271" t="s">
+      <c r="C12" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="271"/>
+      <c r="D12" s="270"/>
       <c r="E12" s="65">
         <v>68</v>
       </c>
@@ -31398,10 +31420,10 @@
       <c r="B19" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C19" s="271" t="s">
+      <c r="C19" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="271"/>
+      <c r="D19" s="270"/>
       <c r="E19" s="65">
         <v>68</v>
       </c>
@@ -31475,7 +31497,7 @@
       <c r="B24" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="250" t="s">
+      <c r="C24" s="249" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="219"/>
@@ -31508,7 +31530,7 @@
       <c r="C26" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="251"/>
+      <c r="D26" s="250"/>
       <c r="E26" s="65">
         <v>0</v>
       </c>
@@ -31551,7 +31573,7 @@
       <c r="B31" s="10"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A32" s="249" t="s">
+      <c r="A32" s="248" t="s">
         <v>104</v>
       </c>
       <c r="B32" s="165"/>
@@ -32098,10 +32120,10 @@
         <v>73</v>
       </c>
       <c r="B89" s="120"/>
-      <c r="C89" s="262" t="s">
+      <c r="C89" s="261" t="s">
         <v>377</v>
       </c>
-      <c r="D89" s="252"/>
+      <c r="D89" s="251"/>
       <c r="E89" s="51">
         <v>150</v>
       </c>
@@ -32118,12 +32140,12 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A91" s="241" t="s">
+      <c r="A91" s="259" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="241"/>
-      <c r="C91" s="245"/>
-      <c r="D91" s="245"/>
+      <c r="B91" s="259"/>
+      <c r="C91" s="244"/>
+      <c r="D91" s="244"/>
       <c r="E91" s="74">
         <f>C84</f>
         <v>1387</v>
@@ -32132,13 +32154,13 @@
     <row r="92" spans="1:8" ht="13.5" customHeight="1">
       <c r="A92" s="72"/>
       <c r="B92" s="72"/>
-      <c r="C92" s="248" t="s">
+      <c r="C92" s="247" t="s">
         <v>41</v>
       </c>
       <c r="D92" s="215"/>
       <c r="E92" s="73">
         <f>('April 2025 - June 2025'!E109+E14)-SUM(E89:E91)</f>
-        <v>803.86999999999989</v>
+        <v>853.86999999999989</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="13.5" customHeight="1"/>
@@ -32182,11 +32204,11 @@
         <v>102</v>
       </c>
       <c r="B96" s="229"/>
-      <c r="C96" s="243"/>
-      <c r="D96" s="244"/>
+      <c r="C96" s="242"/>
+      <c r="D96" s="243"/>
       <c r="E96" s="86">
         <f>E92</f>
-        <v>803.86999999999989</v>
+        <v>853.86999999999989</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="13.5" customHeight="1">
@@ -32197,7 +32219,7 @@
       <c r="C97" s="169" t="s">
         <v>312</v>
       </c>
-      <c r="D97" s="252"/>
+      <c r="D97" s="251"/>
       <c r="E97" s="51">
         <v>0</v>
       </c>
@@ -32218,8 +32240,8 @@
         <v>40</v>
       </c>
       <c r="B99" s="275"/>
-      <c r="C99" s="245"/>
-      <c r="D99" s="251"/>
+      <c r="C99" s="244"/>
+      <c r="D99" s="250"/>
       <c r="E99" s="74">
         <f>C84</f>
         <v>1387</v>
@@ -32232,7 +32254,7 @@
       <c r="D100" s="197"/>
       <c r="E100" s="73">
         <f>(E21+E96)-SUM(E97:E99)</f>
-        <v>389.86999999999989</v>
+        <v>439.86999999999989</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="13.5" customHeight="1">
@@ -32289,11 +32311,11 @@
         <v>105</v>
       </c>
       <c r="B105" s="229"/>
-      <c r="C105" s="263"/>
+      <c r="C105" s="262"/>
       <c r="D105" s="278"/>
       <c r="E105" s="36">
         <f>E100</f>
-        <v>389.86999999999989</v>
+        <v>439.86999999999989</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="13.5" customHeight="1">
@@ -32304,14 +32326,14 @@
       <c r="C106" s="189" t="s">
         <v>312</v>
       </c>
-      <c r="D106" s="256"/>
+      <c r="D106" s="255"/>
       <c r="E106" s="71">
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">
       <c r="A107" s="201"/>
-      <c r="B107" s="268"/>
+      <c r="B107" s="264"/>
       <c r="C107" s="169" t="s">
         <v>320</v>
       </c>
@@ -32325,8 +32347,8 @@
         <v>40</v>
       </c>
       <c r="B108" s="275"/>
-      <c r="C108" s="245"/>
-      <c r="D108" s="251"/>
+      <c r="C108" s="244"/>
+      <c r="D108" s="250"/>
       <c r="E108" s="74">
         <f>C84</f>
         <v>1387</v>
@@ -32339,7 +32361,7 @@
       <c r="D109" s="197"/>
       <c r="E109" s="100">
         <f>(E27+E105)-SUM(E106:E108)</f>
-        <v>1407.87</v>
+        <v>1457.87</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="13.5" customHeight="1">
@@ -36173,7 +36195,7 @@
       </c>
       <c r="C3" s="4">
         <f>E110</f>
-        <v>4583.87</v>
+        <v>4633.87</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -36205,7 +36227,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>4583.87</v>
+        <v>4633.87</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -36355,10 +36377,10 @@
       <c r="B11" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C11" s="271" t="s">
+      <c r="C11" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="271"/>
+      <c r="D11" s="270"/>
       <c r="E11" s="65">
         <v>68</v>
       </c>
@@ -36459,10 +36481,10 @@
       <c r="B18" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C18" s="271" t="s">
+      <c r="C18" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="271"/>
+      <c r="D18" s="270"/>
       <c r="E18" s="65">
         <v>68</v>
       </c>
@@ -36474,10 +36496,10 @@
       <c r="B19" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C19" s="271" t="s">
+      <c r="C19" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="271"/>
+      <c r="D19" s="270"/>
       <c r="E19" s="65">
         <v>68</v>
       </c>
@@ -36551,7 +36573,7 @@
       <c r="B24" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="250" t="s">
+      <c r="C24" s="249" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="219"/>
@@ -36581,10 +36603,10 @@
       <c r="B26" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C26" s="271" t="s">
+      <c r="C26" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="271"/>
+      <c r="D26" s="270"/>
       <c r="E26" s="65">
         <v>68</v>
       </c>
@@ -36599,7 +36621,7 @@
       <c r="C27" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="251"/>
+      <c r="D27" s="250"/>
       <c r="E27" s="65">
         <v>0</v>
       </c>
@@ -36642,7 +36664,7 @@
       <c r="B32" s="10"/>
     </row>
     <row r="33" spans="1:4" ht="13.5" customHeight="1">
-      <c r="A33" s="249" t="s">
+      <c r="A33" s="248" t="s">
         <v>205</v>
       </c>
       <c r="B33" s="165"/>
@@ -37192,7 +37214,7 @@
       <c r="C90" s="169" t="s">
         <v>312</v>
       </c>
-      <c r="D90" s="252"/>
+      <c r="D90" s="251"/>
       <c r="E90" s="51">
         <v>0</v>
       </c>
@@ -37209,12 +37231,12 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A92" s="241" t="s">
+      <c r="A92" s="259" t="s">
         <v>40</v>
       </c>
-      <c r="B92" s="241"/>
-      <c r="C92" s="245"/>
-      <c r="D92" s="245"/>
+      <c r="B92" s="259"/>
+      <c r="C92" s="244"/>
+      <c r="D92" s="244"/>
       <c r="E92" s="74">
         <f>C85</f>
         <v>1387</v>
@@ -37223,13 +37245,13 @@
     <row r="93" spans="1:8" ht="13.5" customHeight="1">
       <c r="A93" s="72"/>
       <c r="B93" s="72"/>
-      <c r="C93" s="248" t="s">
+      <c r="C93" s="247" t="s">
         <v>41</v>
       </c>
       <c r="D93" s="215"/>
       <c r="E93" s="73">
         <f>('July 2025 - September 2025'!E109+E13)-SUM(E90:E92)</f>
-        <v>2493.87</v>
+        <v>2543.87</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1"/>
@@ -37273,11 +37295,11 @@
         <v>202</v>
       </c>
       <c r="B97" s="229"/>
-      <c r="C97" s="263"/>
-      <c r="D97" s="264"/>
+      <c r="C97" s="262"/>
+      <c r="D97" s="263"/>
       <c r="E97" s="36">
         <f>E93</f>
-        <v>2493.87</v>
+        <v>2543.87</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="36.75" customHeight="1">
@@ -37288,14 +37310,14 @@
       <c r="C98" s="277" t="s">
         <v>377</v>
       </c>
-      <c r="D98" s="261"/>
+      <c r="D98" s="269"/>
       <c r="E98" s="51">
         <v>150</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A99" s="268"/>
-      <c r="B99" s="268"/>
+      <c r="A99" s="264"/>
+      <c r="B99" s="264"/>
       <c r="C99" s="162" t="s">
         <v>320</v>
       </c>
@@ -37323,7 +37345,7 @@
       <c r="D101" s="166"/>
       <c r="E101" s="36">
         <f>(E21+E97)-SUM(E98:E100)</f>
-        <v>3497.87</v>
+        <v>3547.87</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="13.5" customHeight="1">
@@ -37384,7 +37406,7 @@
       <c r="D106" s="166"/>
       <c r="E106" s="36">
         <f>E101</f>
-        <v>3497.87</v>
+        <v>3547.87</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">
@@ -37401,8 +37423,8 @@
       </c>
     </row>
     <row r="108" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A108" s="268"/>
-      <c r="B108" s="268"/>
+      <c r="A108" s="264"/>
+      <c r="B108" s="264"/>
       <c r="C108" s="162" t="s">
         <v>320</v>
       </c>
@@ -37430,7 +37452,7 @@
       <c r="D110" s="166"/>
       <c r="E110" s="51">
         <f>(E28+E106)-SUM(E107:E109)</f>
-        <v>4583.87</v>
+        <v>4633.87</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="13.5" customHeight="1">
@@ -41266,7 +41288,7 @@
       </c>
       <c r="C3" s="4">
         <f>E109</f>
-        <v>7691.869999999999</v>
+        <v>7741.869999999999</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -41298,7 +41320,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>7691.869999999999</v>
+        <v>7741.869999999999</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -41448,10 +41470,10 @@
       <c r="B11" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C11" s="271" t="s">
+      <c r="C11" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="271"/>
+      <c r="D11" s="270"/>
       <c r="E11" s="65">
         <v>68</v>
       </c>
@@ -41552,10 +41574,10 @@
       <c r="B18" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C18" s="271" t="s">
+      <c r="C18" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="271"/>
+      <c r="D18" s="270"/>
       <c r="E18" s="65">
         <v>68</v>
       </c>
@@ -41629,7 +41651,7 @@
       <c r="B23" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="250" t="s">
+      <c r="C23" s="249" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="219"/>
@@ -41659,10 +41681,10 @@
       <c r="B25" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C25" s="271" t="s">
+      <c r="C25" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="271"/>
+      <c r="D25" s="270"/>
       <c r="E25" s="65">
         <v>68</v>
       </c>
@@ -41677,7 +41699,7 @@
       <c r="C26" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="251"/>
+      <c r="D26" s="250"/>
       <c r="E26" s="65">
         <v>0</v>
       </c>
@@ -41720,7 +41742,7 @@
       <c r="B31" s="10"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A32" s="249" t="s">
+      <c r="A32" s="248" t="s">
         <v>228</v>
       </c>
       <c r="B32" s="165"/>
@@ -42267,10 +42289,10 @@
         <v>73</v>
       </c>
       <c r="B89" s="157"/>
-      <c r="C89" s="262" t="s">
+      <c r="C89" s="261" t="s">
         <v>377</v>
       </c>
-      <c r="D89" s="252"/>
+      <c r="D89" s="251"/>
       <c r="E89" s="51">
         <v>150</v>
       </c>
@@ -42287,12 +42309,12 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A91" s="241" t="s">
+      <c r="A91" s="259" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="241"/>
-      <c r="C91" s="245"/>
-      <c r="D91" s="245"/>
+      <c r="B91" s="259"/>
+      <c r="C91" s="244"/>
+      <c r="D91" s="244"/>
       <c r="E91" s="74">
         <f>C84</f>
         <v>1387</v>
@@ -42301,13 +42323,13 @@
     <row r="92" spans="1:8" ht="13.5" customHeight="1">
       <c r="A92" s="72"/>
       <c r="B92" s="72"/>
-      <c r="C92" s="248" t="s">
+      <c r="C92" s="247" t="s">
         <v>41</v>
       </c>
       <c r="D92" s="215"/>
       <c r="E92" s="73">
         <f>('October 2025 - December 2025'!E110+E13)-SUM(E89:E91)</f>
-        <v>5519.87</v>
+        <v>5569.87</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="13.5" customHeight="1"/>
@@ -42351,11 +42373,11 @@
         <v>100</v>
       </c>
       <c r="B96" s="229"/>
-      <c r="C96" s="263"/>
-      <c r="D96" s="264"/>
+      <c r="C96" s="262"/>
+      <c r="D96" s="263"/>
       <c r="E96" s="36">
         <f>E92</f>
-        <v>5519.87</v>
+        <v>5569.87</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="13.5" customHeight="1">
@@ -42366,14 +42388,14 @@
       <c r="C97" s="187" t="s">
         <v>312</v>
       </c>
-      <c r="D97" s="261"/>
+      <c r="D97" s="269"/>
       <c r="E97" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A98" s="268"/>
-      <c r="B98" s="268"/>
+      <c r="A98" s="264"/>
+      <c r="B98" s="264"/>
       <c r="C98" s="162" t="s">
         <v>320</v>
       </c>
@@ -42401,7 +42423,7 @@
       <c r="D100" s="166"/>
       <c r="E100" s="36">
         <f>(E20+E96)-SUM(E97:E99)</f>
-        <v>6605.87</v>
+        <v>6655.87</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="13.5" customHeight="1">
@@ -42462,7 +42484,7 @@
       <c r="D105" s="166"/>
       <c r="E105" s="36">
         <f>E100</f>
-        <v>6605.87</v>
+        <v>6655.87</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="13.5" customHeight="1">
@@ -42479,8 +42501,8 @@
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A107" s="268"/>
-      <c r="B107" s="268"/>
+      <c r="A107" s="264"/>
+      <c r="B107" s="264"/>
       <c r="C107" s="162" t="s">
         <v>320</v>
       </c>
@@ -42508,7 +42530,7 @@
       <c r="D109" s="166"/>
       <c r="E109" s="51">
         <f>(E27+E105)-SUM(E106:E108)</f>
-        <v>7691.869999999999</v>
+        <v>7741.869999999999</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="13.5" customHeight="1">
@@ -46343,7 +46365,7 @@
       </c>
       <c r="C3" s="4">
         <f>E109</f>
-        <v>10799.869999999999</v>
+        <v>10849.869999999999</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -46375,7 +46397,7 @@
       </c>
       <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
-        <v>10799.869999999999</v>
+        <v>10849.869999999999</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -46525,10 +46547,10 @@
       <c r="B11" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C11" s="271" t="s">
+      <c r="C11" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="271"/>
+      <c r="D11" s="270"/>
       <c r="E11" s="65">
         <v>68</v>
       </c>
@@ -46629,10 +46651,10 @@
       <c r="B18" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C18" s="271" t="s">
+      <c r="C18" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="271"/>
+      <c r="D18" s="270"/>
       <c r="E18" s="65">
         <v>68</v>
       </c>
@@ -46706,7 +46728,7 @@
       <c r="B23" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="250" t="s">
+      <c r="C23" s="249" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="219"/>
@@ -46736,10 +46758,10 @@
       <c r="B25" s="31" t="s">
         <v>379</v>
       </c>
-      <c r="C25" s="271" t="s">
+      <c r="C25" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="271"/>
+      <c r="D25" s="270"/>
       <c r="E25" s="65">
         <v>68</v>
       </c>
@@ -46754,7 +46776,7 @@
       <c r="C26" s="154" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="251"/>
+      <c r="D26" s="250"/>
       <c r="E26" s="65">
         <v>0</v>
       </c>
@@ -46797,7 +46819,7 @@
       <c r="B31" s="10"/>
     </row>
     <row r="32" spans="1:25" ht="13.5" customHeight="1">
-      <c r="A32" s="249" t="s">
+      <c r="A32" s="248" t="s">
         <v>241</v>
       </c>
       <c r="B32" s="165"/>
@@ -47344,10 +47366,10 @@
         <v>73</v>
       </c>
       <c r="B89" s="157"/>
-      <c r="C89" s="262" t="s">
+      <c r="C89" s="261" t="s">
         <v>377</v>
       </c>
-      <c r="D89" s="252"/>
+      <c r="D89" s="251"/>
       <c r="E89" s="51">
         <v>150</v>
       </c>
@@ -47364,12 +47386,12 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A91" s="255" t="s">
+      <c r="A91" s="254" t="s">
         <v>40</v>
       </c>
       <c r="B91" s="272"/>
-      <c r="C91" s="245"/>
-      <c r="D91" s="245"/>
+      <c r="C91" s="244"/>
+      <c r="D91" s="244"/>
       <c r="E91" s="74">
         <f>C84</f>
         <v>1387</v>
@@ -47378,13 +47400,13 @@
     <row r="92" spans="1:8" ht="13.5" customHeight="1">
       <c r="A92" s="72"/>
       <c r="B92" s="72"/>
-      <c r="C92" s="248" t="s">
+      <c r="C92" s="247" t="s">
         <v>41</v>
       </c>
       <c r="D92" s="215"/>
       <c r="E92" s="73">
         <f>('January 2026 - March 2026'!E109+E13)-SUM(E89:E91)</f>
-        <v>8627.869999999999</v>
+        <v>8677.869999999999</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="13.5" customHeight="1"/>
@@ -47428,11 +47450,11 @@
         <v>98</v>
       </c>
       <c r="B96" s="229"/>
-      <c r="C96" s="263"/>
-      <c r="D96" s="264"/>
+      <c r="C96" s="262"/>
+      <c r="D96" s="263"/>
       <c r="E96" s="36">
         <f>E92</f>
-        <v>8627.869999999999</v>
+        <v>8677.869999999999</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="13.5" customHeight="1">
@@ -47443,14 +47465,14 @@
       <c r="C97" s="187" t="s">
         <v>312</v>
       </c>
-      <c r="D97" s="261"/>
+      <c r="D97" s="269"/>
       <c r="E97" s="51">
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A98" s="268"/>
-      <c r="B98" s="268"/>
+      <c r="A98" s="264"/>
+      <c r="B98" s="264"/>
       <c r="C98" s="162" t="s">
         <v>320</v>
       </c>
@@ -47478,7 +47500,7 @@
       <c r="D100" s="166"/>
       <c r="E100" s="36">
         <f>(E20+E96)-SUM(E97:E99)</f>
-        <v>9713.869999999999</v>
+        <v>9763.869999999999</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="13.5" customHeight="1">
@@ -47539,7 +47561,7 @@
       <c r="D105" s="166"/>
       <c r="E105" s="36">
         <f>E100</f>
-        <v>9713.869999999999</v>
+        <v>9763.869999999999</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="13.5" customHeight="1">
@@ -47556,8 +47578,8 @@
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A107" s="268"/>
-      <c r="B107" s="268"/>
+      <c r="A107" s="264"/>
+      <c r="B107" s="264"/>
       <c r="C107" s="162" t="s">
         <v>320</v>
       </c>
@@ -47585,7 +47607,7 @@
       <c r="D109" s="166"/>
       <c r="E109" s="51">
         <f>(E27+E105)-SUM(E106:E108)</f>
-        <v>10799.869999999999</v>
+        <v>10849.869999999999</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="13.5" customHeight="1">

</xml_diff>